<commit_message>
star, user 기능 완료
</commit_message>
<xml_diff>
--- a/exerdProject/기능명세서.xlsx
+++ b/exerdProject/기능명세서.xlsx
@@ -21,15 +21,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="305">
   <si>
     <t>select MEM_ID, MEM_NICK, MEM_NM from MEM_TBL limit 10 offset N;</t>
   </si>
   <si>
     <t>select M.MEM_ID, M.MEM_NICK, M.MEM_NM, M.MEM_STAT, M.ACVT, F.FILE_PATH from MEM_TBL M inner join FILE_TBL F on M.FILE_IDX = F.FILE_IDX where M.MEM_ID = '아이디';</t>
-  </si>
-  <si>
-    <t>update MEM_TBL M LEFT OUTER JOIN FILE_TBL F ON M.FILE_IDX = F.FILE_IDX SET M.MEM_PWD = hex(aes_encrypt('암호 문자열', '암호화 키')), M.MEM_NICK = '닉네임', M.MEM_NM = '이름', F.FILE_PATH = '파일경로' where M.MEM_ID = '아이디';</t>
   </si>
   <si>
     <t>select M.MEM_ID, M.MEM_NICK, M.MEM_NM, M.MEM_STAT, F.FILE_PATH from MEM_TBL M inner join FILE_TBL F on M.FILE_IDX = F.FILE_IDX where M.MEM_ID = 'ID' and M.ACVT = TRUE and M.MEM_PWD = hex(aes_encrypt('PWD', '암호화 키'));</t>
@@ -38,28 +35,13 @@
     <t>select S.STAR_IDX, S.STAR_NM, S.STAR_TYP, S.STAR_DBT_DATE, S.CMPY_NM, F.FILE_PATH FROM STAR_TBL S inner join FILE_TBL F on S.FILE_IDX = F.FILE_IDX limit 10 offset N;</t>
   </si>
   <si>
-    <t>select S.STAR_MEM_IDX, S.STAR_MEM_HGHT, S.STAR_MEM_AGE, S.STAR_MEM_BLD, S.STAR_MEM_WGHT, S.STAR_MEM_BIRTH, GS.STAR_NM, GS.STAR_TYP from STAR_MEM_TBL S right outer join GRP_TBL G on S.GRP_IDX = G.GRP_IDX right outer join STAR_TBL GS on G.STAR_IDX = GS.STAR_IDX where S.STAR_IDX = '인덱스' and GS.STAR_TYP='TYP';</t>
-  </si>
-  <si>
     <t>select G.GRP_IDX, G.CLB_SITE from GRP_TBL G inner join STAR_TBL S on G.STAR_IDX = S.STAR_IDX where G.STAR_IDX = '인덱스';</t>
-  </si>
-  <si>
-    <t>update STAR_MEM_TBL SM inner join STAR_TBL SI on SM.STAR_IDX = SI.STAR_IDX inner join FILE_TBL FT on SM.FILE_IDX = FT.FILE_IDX set SM.STAR_MEM_HGHT = '키', SM.STAR_MEM_BLD = '혈액형', SM.STAR_MEM_WGHT = '몸무게', SM.STAR_MEM_BIRTH = '출생', SI.STAR_DBT_DATE = '데뷔날짜', FT.FILE_PATH = '파일경로', SM.GRP_IDX = (select * from (select G.GRP_IDX from GRP_TBL G inner join STAR_TBL S on G.STAR_IDX = S.STAR_IDX where S.STAR_NM = '그룹이름' and S.STAR_TYP = 'GRP')T) where SM.STAR_MEM_IDX = '인덱스' and SI.STAR_TYP = 'STAR';</t>
-  </si>
-  <si>
-    <t>update GRP_TBL GT inner join STAR_TBL ST on GT.STAR_IDX = ST.STAR_IDX inner join FILE_TBL FT on ST.FILE_IDX = FT.FILE_IDX set CLB_SITE = '사이트', ST.STAR_DBT_DATE = '데뷔날짜', FT.FILE_PATH = '파일 경로' where GT.GRP_IDX = '그룹인덱스';</t>
-  </si>
-  <si>
-    <t>delete ST, SMT, FT from STAR_TBL ST inner join STAR_MEM_TBL SMT on ST.STAR_IDX = SMT.STAR_IDX inner join FILE_TBL FT on ST.FILE_IDX = FT.FILE_IDX where ST.STAR_IDX = '인덱스';</t>
   </si>
   <si>
     <t>delete ST, GT, FT from STAR_TBL ST inner join GRP_TBL GT on ST.STAR_IDX = GT.SRP_IDX inner join FILE_TBL FT on ST.FILE_IDX = FT.FILE_IDX where ST.GRP_IDX = '그룹인덱스';</t>
   </si>
   <si>
     <t>insert into LIKE_STAR_TBL(STAR_IDX, MEM_ID) values ('연예인인덱스', '회원아이디');</t>
-  </si>
-  <si>
-    <t>insert into STAR_TAG_TBL(STAR_IDX, TAG_NM) values ('연예인인덱스', '태그이름');</t>
   </si>
   <si>
     <t>select C.CMPY_NM, C.CMPY_REP, F.FILE_PATH from CMPY_TBL C inner join FILE_TBL F on C.FILE_IDX = F.FILE_IDX LIMIT 10 OFFSET N;</t>
@@ -10847,9 +10829,6 @@
     <t>insert into FILE_TBL(FILE_NM, FILE_PATH, FILE_CRT_DATE) values ('이름', '경로',SYSDATE()); insert into MEM_TBL ( MEM_ID, MEM_PWD, MEM_NICK, MEM_NM, FILE_IDX) values ('아이디', hex(aes_encrypt('암호 문자열', '암호화 키')), '닉네임', '이름', LAST_INSERT_ID());</t>
   </si>
   <si>
-    <t>insert into FILE_TBL(FILE_NM, FILE_PATH, FILE_CRT_DATE) values ('파일이름', '파일경로', SYSDATE()); insert into STAR_TBL(STAR_NM, STAR_TYP, STAR_DBT_DATE, CMPY_NM, FILE_IDX) values ('이름', 'GRP', SYSDATE(), '소속사', LAST_INSERT_ID()); insert into GRP_TBL(STAR_IDX, CLB_SITE) values (LAST_INSERT_ID(), '사이트');</t>
-  </si>
-  <si>
     <t>crt_mem</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -11071,6 +11050,38 @@
   </si>
   <si>
     <t>**/*/do : 뷰가 아닌 동작 url</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into FILE_TBL(FILE_NM, FILE_PATH, FILE_CRT_DATE) values ('파일이름', '파일경로', SYSDATE()); insert into STAR_TBL(STAR_NM, STAR_TYP, STAR_DBT_DATE, CMPY_NM, FILE_IDX) values ('이름', 'GRP', SYSDATE(), '소속사', LAST_INSERT_ID()); insert into GRP_TBL(STAR_IDX, CLB_SITE) values (LAST_INSERT_ID(), '사이트');</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select S.STAR_MEM_IDX, S.STAR_MEM_HGHT, S.STAR_MEM_AGE, S.STAR_MEM_BLD, S.STAR_MEM_WGHT, S.STAR_MEM_BIRTH, GS.STAR_NM, GS.STAR_TYP from STAR_MEM_TBL S right outer join GRP_TBL G on S.GRP_IDX = G.GRP_IDX right outer join STAR_TBL GS on G.STAR_IDX = GS.STAR_IDX where S.STAR_IDX = '인덱스' and GS.STAR_TYP='TYP';</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>**/*.admin: 관리자 확인이 필요한 url</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>update STAR_MEM_TBL SM inner join STAR_TBL SI on SM.STAR_IDX = SI.STAR_IDX inner join FILE_TBL FT on SM.FILE_IDX = FT.FILE_IDX set SM.STAR_MEM_HGHT = '키', SM.STAR_MEM_BLD = '혈액형', SM.STAR_MEM_WGHT = '몸무게', SM.STAR_MEM_BIRTH = '출생', SI.STAR_DBT_DATE = '데뷔날짜', FT.FILE_NM = '파일이름', FT.FILE_PATH = '파일경로', SM.GRP_IDX = (select * from (select G.GRP_IDX from GRP_TBL G inner join STAR_TBL S on G.STAR_IDX = S.STAR_IDX where S.STAR_NM = '그룹이름' and S.STAR_TYP = 'GRP')T) where SM.STAR_MEM_IDX = '인덱스' and SI.STAR_TYP = 'STAR';</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>update GRP_TBL GT inner join STAR_TBL ST on GT.STAR_IDX = ST.STAR_IDX inner join FILE_TBL FT on ST.FILE_IDX = FT.FILE_IDX set CLB_SITE = '사이트', ST.STAR_DBT_DATE = '데뷔날짜', FT.FILE_NM = '파일이름', FT.FILE_PATH = '파일 경로' where GT.GRP_IDX = '그룹인덱스';</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>update MEM_TBL M LEFT OUTER JOIN FILE_TBL F ON M.FILE_IDX = F.FILE_IDX SET M.MEM_PWD = hex(aes_encrypt('암호 문자열', '암호화 키')), M.MEM_NICK = '닉네임', M.MEM_NM = '이름', F.FILE_NM = '파일 이름', F.FILE_PATH = '파일경로' where M.MEM_ID = '아이디';</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>delete ST, SMT, FT from STAR_TBL ST inner join STAR_MEM_TBL SMT on ST.STAR_IDX = SMT.STAR_IDX inner join FILE_TBL FT on ST.FILE_IDX = FT.FILE_IDX where SMT.STAR_MEM_IDX = '인덱스';</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into STAR_TAG_TBL(STAR_IDX, TAG_NM) values ('연예인인덱스', '태그이름');</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -11361,6 +11372,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -11382,7 +11394,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -11448,7 +11459,7 @@
         <xdr:cNvPr id="3" name="그림 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{72F30C73-F9FC-4F38-BA21-6FBBC4E49CDB}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72F30C73-F9FC-4F38-BA21-6FBBC4E49CDB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11498,7 +11509,7 @@
         <xdr:cNvPr id="5" name="그림 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5BB94D47-326F-4819-8971-AA13705ADEA4}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5BB94D47-326F-4819-8971-AA13705ADEA4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11548,7 +11559,7 @@
         <xdr:cNvPr id="7" name="그림 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{59C13640-91FA-4E80-824E-E4D9C44B5BED}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59C13640-91FA-4E80-824E-E4D9C44B5BED}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11598,7 +11609,7 @@
         <xdr:cNvPr id="9" name="그림 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C4A3605E-7644-45D4-8DE6-84FD004B3F4C}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4A3605E-7644-45D4-8DE6-84FD004B3F4C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11648,7 +11659,7 @@
         <xdr:cNvPr id="11" name="그림 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{62DD966B-C63A-459D-B9C1-C4D087351D8E}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62DD966B-C63A-459D-B9C1-C4D087351D8E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11698,7 +11709,7 @@
         <xdr:cNvPr id="13" name="그림 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A1FEB21B-F265-43E5-BC0F-5A5C3072778D}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1FEB21B-F265-43E5-BC0F-5A5C3072778D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11748,7 +11759,7 @@
         <xdr:cNvPr id="15" name="그림 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{82167F25-CE0C-4328-B74B-67C4A9238083}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82167F25-CE0C-4328-B74B-67C4A9238083}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11798,7 +11809,7 @@
         <xdr:cNvPr id="17" name="그림 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F83AB63C-A07B-4B7E-AB95-B45645F50602}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F83AB63C-A07B-4B7E-AB95-B45645F50602}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11848,7 +11859,7 @@
         <xdr:cNvPr id="19" name="그림 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{433948DD-2AD1-4AC9-B842-63A78A067A70}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{433948DD-2AD1-4AC9-B842-63A78A067A70}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11898,7 +11909,7 @@
         <xdr:cNvPr id="21" name="그림 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{082B1200-C085-4FA7-BE82-27A6BEA6E852}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{082B1200-C085-4FA7-BE82-27A6BEA6E852}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11948,7 +11959,7 @@
         <xdr:cNvPr id="23" name="그림 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E7A074D7-8F92-4F0A-8B56-B91E2CBC3825}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7A074D7-8F92-4F0A-8B56-B91E2CBC3825}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11998,7 +12009,7 @@
         <xdr:cNvPr id="25" name="그림 24">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{53A77203-91F8-463E-8B1B-039C3269D532}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53A77203-91F8-463E-8B1B-039C3269D532}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12048,7 +12059,7 @@
         <xdr:cNvPr id="27" name="그림 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C7118837-89E4-446F-97EF-B5D9FB7F2FB4}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7118837-89E4-446F-97EF-B5D9FB7F2FB4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12098,7 +12109,7 @@
         <xdr:cNvPr id="29" name="그림 28">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8737BCA7-F78B-4B91-A595-9653D635C7D5}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8737BCA7-F78B-4B91-A595-9653D635C7D5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12148,7 +12159,7 @@
         <xdr:cNvPr id="31" name="그림 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B2AF5EE9-C4ED-4408-A5F6-28A0E9417D7E}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2AF5EE9-C4ED-4408-A5F6-28A0E9417D7E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12198,7 +12209,7 @@
         <xdr:cNvPr id="33" name="그림 32">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6B138BD1-1A05-4487-B0A5-BADA3B2BF1C1}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B138BD1-1A05-4487-B0A5-BADA3B2BF1C1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12248,7 +12259,7 @@
         <xdr:cNvPr id="35" name="그림 34">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B8EEEE74-6CDD-4AD0-AA9E-B9957525B74B}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8EEEE74-6CDD-4AD0-AA9E-B9957525B74B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12298,7 +12309,7 @@
         <xdr:cNvPr id="37" name="그림 36">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E3433636-4576-43A7-8AD9-BB8E1A1E1AD8}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3433636-4576-43A7-8AD9-BB8E1A1E1AD8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12348,7 +12359,7 @@
         <xdr:cNvPr id="39" name="그림 38">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3C4A0C2B-4389-4D57-A3E0-2D04338083F9}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C4A0C2B-4389-4D57-A3E0-2D04338083F9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12398,7 +12409,7 @@
         <xdr:cNvPr id="41" name="그림 40">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{89BC0C82-65FA-44E5-A832-010C0FF640FC}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89BC0C82-65FA-44E5-A832-010C0FF640FC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12448,7 +12459,7 @@
         <xdr:cNvPr id="43" name="그림 42">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{31F9904A-3271-4FA6-8901-1D90AB0455FB}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31F9904A-3271-4FA6-8901-1D90AB0455FB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12498,7 +12509,7 @@
         <xdr:cNvPr id="45" name="그림 44">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0683093B-4E9B-475F-811C-7650A098856C}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0683093B-4E9B-475F-811C-7650A098856C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12548,7 +12559,7 @@
         <xdr:cNvPr id="47" name="그림 46">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2009715D-AB1E-470A-AA53-9931BA579CDC}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2009715D-AB1E-470A-AA53-9931BA579CDC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12598,7 +12609,7 @@
         <xdr:cNvPr id="49" name="그림 48">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{18FFBF34-399E-4097-A49B-AAEB71760605}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18FFBF34-399E-4097-A49B-AAEB71760605}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12648,7 +12659,7 @@
         <xdr:cNvPr id="51" name="그림 50">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D6310A5F-8868-44D1-AD9B-A1998B7650F4}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6310A5F-8868-44D1-AD9B-A1998B7650F4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12938,7 +12949,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -12946,10 +12957,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA1012"/>
+  <dimension ref="A1:AA1013"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="17"/>
@@ -12964,107 +12975,74 @@
   <sheetData>
     <row r="1" spans="1:27">
       <c r="B1" s="19" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="C1" s="4"/>
     </row>
     <row r="2" spans="1:27">
       <c r="B2" s="19" t="s">
-        <v>302</v>
-      </c>
+        <v>299</v>
+      </c>
+      <c r="C2" s="4"/>
     </row>
     <row r="3" spans="1:27">
       <c r="B3" s="19" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" s="44" customFormat="1">
-      <c r="A4" s="19"/>
-      <c r="B4" s="44" t="s">
-        <v>301</v>
-      </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="34"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="19"/>
-      <c r="O4" s="19"/>
-      <c r="P4" s="19"/>
-      <c r="Q4" s="19"/>
-      <c r="R4" s="19"/>
-      <c r="S4" s="19"/>
-      <c r="T4" s="19"/>
-      <c r="U4" s="19"/>
-      <c r="V4" s="19"/>
-      <c r="W4" s="19"/>
-      <c r="X4" s="19"/>
-      <c r="Y4" s="19"/>
-      <c r="Z4" s="19"/>
-      <c r="AA4" s="19"/>
-    </row>
-    <row r="5" spans="1:27" ht="17.399999999999999" customHeight="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="40"/>
-      <c r="J5" s="40"/>
-      <c r="K5" s="32"/>
+        <v>295</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27">
+      <c r="B4" s="19" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" s="37" customFormat="1">
+      <c r="A5" s="19"/>
+      <c r="B5" s="37" t="s">
+        <v>294</v>
+      </c>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="34"/>
       <c r="L5" s="19"/>
       <c r="M5" s="19"/>
       <c r="N5" s="19"/>
       <c r="O5" s="19"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="3"/>
-      <c r="S5" s="3"/>
-      <c r="T5" s="3"/>
-      <c r="U5" s="3"/>
-      <c r="V5" s="3"/>
-      <c r="W5" s="3"/>
-      <c r="X5" s="3"/>
-      <c r="Y5" s="3"/>
-      <c r="Z5" s="3"/>
-      <c r="AA5" s="3"/>
+      <c r="P5" s="19"/>
+      <c r="Q5" s="19"/>
+      <c r="R5" s="19"/>
+      <c r="S5" s="19"/>
+      <c r="T5" s="19"/>
+      <c r="U5" s="19"/>
+      <c r="V5" s="19"/>
+      <c r="W5" s="19"/>
+      <c r="X5" s="19"/>
+      <c r="Y5" s="19"/>
+      <c r="Z5" s="19"/>
+      <c r="AA5" s="19"/>
     </row>
     <row r="6" spans="1:27" ht="17.399999999999999" customHeight="1">
       <c r="A6" s="3"/>
-      <c r="B6" s="40"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="40"/>
-      <c r="J6" s="40"/>
-      <c r="K6" s="33" t="s">
-        <v>255</v>
-      </c>
-      <c r="L6" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="M6" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="N6" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="O6" s="23" t="s">
-        <v>21</v>
-      </c>
+      <c r="B6" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="32"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19"/>
+      <c r="O6" s="19"/>
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
       <c r="R6" s="3"/>
@@ -13078,24 +13056,32 @@
       <c r="Z6" s="3"/>
       <c r="AA6" s="3"/>
     </row>
-    <row r="7" spans="1:27" ht="18" customHeight="1">
+    <row r="7" spans="1:27" ht="17.399999999999999" customHeight="1">
       <c r="A7" s="3"/>
-      <c r="B7" s="40"/>
-      <c r="C7" s="40"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="40"/>
-      <c r="J7" s="40"/>
-      <c r="K7" s="32"/>
-      <c r="L7" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="M7" s="19"/>
-      <c r="N7" s="19"/>
-      <c r="O7" s="19"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="41"/>
+      <c r="K7" s="33" t="s">
+        <v>248</v>
+      </c>
+      <c r="L7" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="M7" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="N7" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="O7" s="23" t="s">
+        <v>15</v>
+      </c>
       <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
       <c r="R7" s="3"/>
@@ -13111,30 +13097,18 @@
     </row>
     <row r="8" spans="1:27" ht="18" customHeight="1">
       <c r="A8" s="3"/>
-      <c r="B8" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="39"/>
-      <c r="D8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="I8" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="J8" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="K8" s="34" t="s">
-        <v>248</v>
-      </c>
-      <c r="L8" s="5" t="s">
-        <v>246</v>
+      <c r="B8" s="41"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="32"/>
+      <c r="L8" s="19" t="s">
+        <v>16</v>
       </c>
       <c r="M8" s="19"/>
       <c r="N8" s="19"/>
@@ -13152,30 +13126,32 @@
       <c r="Z8" s="3"/>
       <c r="AA8" s="3"/>
     </row>
-    <row r="9" spans="1:27">
+    <row r="9" spans="1:27" ht="18" customHeight="1">
       <c r="A9" s="3"/>
-      <c r="B9" s="39"/>
-      <c r="C9" s="39"/>
+      <c r="B9" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="40"/>
       <c r="D9" s="1" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E9" s="24"/>
       <c r="F9" s="24"/>
       <c r="G9" s="24"/>
-      <c r="H9" s="26" t="s">
-        <v>25</v>
+      <c r="H9" s="25" t="s">
+        <v>19</v>
       </c>
       <c r="I9" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="J9" s="25" t="s">
-        <v>27</v>
+        <v>20</v>
+      </c>
+      <c r="J9" s="26" t="s">
+        <v>21</v>
       </c>
       <c r="K9" s="34" t="s">
-        <v>257</v>
-      </c>
-      <c r="L9" s="6" t="s">
-        <v>0</v>
+        <v>241</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>240</v>
       </c>
       <c r="M9" s="19"/>
       <c r="N9" s="19"/>
@@ -13195,28 +13171,28 @@
     </row>
     <row r="10" spans="1:27">
       <c r="A10" s="3"/>
-      <c r="B10" s="39"/>
-      <c r="C10" s="39"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="40"/>
       <c r="D10" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="E10" s="24"/>
       <c r="F10" s="24"/>
       <c r="G10" s="24"/>
       <c r="H10" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="I10" s="27" t="s">
-        <v>26</v>
+        <v>19</v>
+      </c>
+      <c r="I10" s="25" t="s">
+        <v>20</v>
       </c>
       <c r="J10" s="25" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="K10" s="34" t="s">
-        <v>256</v>
-      </c>
-      <c r="L10" s="5" t="s">
-        <v>1</v>
+        <v>250</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>0</v>
       </c>
       <c r="M10" s="19"/>
       <c r="N10" s="19"/>
@@ -13236,28 +13212,28 @@
     </row>
     <row r="11" spans="1:27">
       <c r="A11" s="3"/>
-      <c r="B11" s="39"/>
-      <c r="C11" s="39"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="40"/>
       <c r="D11" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E11" s="24"/>
       <c r="F11" s="24"/>
       <c r="G11" s="24"/>
-      <c r="H11" s="27" t="s">
-        <v>25</v>
+      <c r="H11" s="26" t="s">
+        <v>19</v>
       </c>
       <c r="I11" s="27" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="J11" s="25" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="K11" s="34" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M11" s="19"/>
       <c r="N11" s="19"/>
@@ -13277,28 +13253,28 @@
     </row>
     <row r="12" spans="1:27">
       <c r="A12" s="3"/>
-      <c r="B12" s="39"/>
-      <c r="C12" s="39"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="40"/>
       <c r="D12" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E12" s="24"/>
       <c r="F12" s="24"/>
       <c r="G12" s="24"/>
-      <c r="H12" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="I12" s="26" t="s">
-        <v>26</v>
+      <c r="H12" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="I12" s="27" t="s">
+        <v>20</v>
       </c>
       <c r="J12" s="25" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="K12" s="34" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>99</v>
+        <v>302</v>
       </c>
       <c r="M12" s="19"/>
       <c r="N12" s="19"/>
@@ -13318,28 +13294,28 @@
     </row>
     <row r="13" spans="1:27">
       <c r="A13" s="3"/>
-      <c r="B13" s="39"/>
-      <c r="C13" s="39"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="40"/>
       <c r="D13" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E13" s="24"/>
       <c r="F13" s="24"/>
       <c r="G13" s="24"/>
-      <c r="H13" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="I13" s="27" t="s">
-        <v>26</v>
+      <c r="H13" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" s="26" t="s">
+        <v>20</v>
       </c>
       <c r="J13" s="25" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="K13" s="34" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>299</v>
+        <v>93</v>
       </c>
       <c r="M13" s="19"/>
       <c r="N13" s="19"/>
@@ -13359,28 +13335,28 @@
     </row>
     <row r="14" spans="1:27">
       <c r="A14" s="3"/>
-      <c r="B14" s="39"/>
-      <c r="C14" s="39"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="40"/>
       <c r="D14" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E14" s="24"/>
       <c r="F14" s="24"/>
       <c r="G14" s="24"/>
       <c r="H14" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="I14" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="J14" s="26" t="s">
-        <v>27</v>
+        <v>19</v>
+      </c>
+      <c r="I14" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="J14" s="25" t="s">
+        <v>21</v>
       </c>
       <c r="K14" s="34" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>3</v>
+        <v>292</v>
       </c>
       <c r="M14" s="19"/>
       <c r="N14" s="19"/>
@@ -13400,25 +13376,29 @@
     </row>
     <row r="15" spans="1:27">
       <c r="A15" s="3"/>
-      <c r="B15" s="39"/>
-      <c r="C15" s="39"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="40"/>
       <c r="D15" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E15" s="24"/>
       <c r="F15" s="24"/>
       <c r="G15" s="24"/>
-      <c r="H15" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="I15" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="J15" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="K15" s="34"/>
-      <c r="L15" s="19"/>
+      <c r="H15" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="I15" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="J15" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="K15" s="34" t="s">
+        <v>254</v>
+      </c>
+      <c r="L15" s="5" t="s">
+        <v>2</v>
+      </c>
       <c r="M15" s="19"/>
       <c r="N15" s="19"/>
       <c r="O15" s="19"/>
@@ -13435,33 +13415,27 @@
       <c r="Z15" s="3"/>
       <c r="AA15" s="3"/>
     </row>
-    <row r="16" spans="1:27" ht="17.399999999999999" customHeight="1">
+    <row r="16" spans="1:27">
       <c r="A16" s="3"/>
-      <c r="B16" s="41" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="41"/>
-      <c r="D16" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
       <c r="H16" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="I16" s="25" t="s">
-        <v>26</v>
+        <v>19</v>
+      </c>
+      <c r="I16" s="26" t="s">
+        <v>20</v>
       </c>
       <c r="J16" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="K16" s="34" t="s">
-        <v>249</v>
-      </c>
-      <c r="L16" s="5" t="s">
-        <v>295</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="K16" s="34"/>
+      <c r="L16" s="19"/>
       <c r="M16" s="19"/>
       <c r="N16" s="19"/>
       <c r="O16" s="19"/>
@@ -13478,30 +13452,32 @@
       <c r="Z16" s="3"/>
       <c r="AA16" s="3"/>
     </row>
-    <row r="17" spans="1:27">
+    <row r="17" spans="1:27" ht="17.399999999999999" customHeight="1">
       <c r="A17" s="3"/>
-      <c r="B17" s="41"/>
-      <c r="C17" s="41"/>
+      <c r="B17" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="42"/>
       <c r="D17" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E17" s="28"/>
       <c r="F17" s="28"/>
       <c r="G17" s="28"/>
       <c r="H17" s="26" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="I17" s="25" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="J17" s="25" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="K17" s="34" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>247</v>
+        <v>288</v>
       </c>
       <c r="M17" s="19"/>
       <c r="N17" s="19"/>
@@ -13521,28 +13497,28 @@
     </row>
     <row r="18" spans="1:27">
       <c r="A18" s="3"/>
-      <c r="B18" s="41"/>
-      <c r="C18" s="41"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="42"/>
       <c r="D18" s="2" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="E18" s="28"/>
       <c r="F18" s="28"/>
       <c r="G18" s="28"/>
       <c r="H18" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="I18" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="J18" s="26" t="s">
-        <v>27</v>
+        <v>19</v>
+      </c>
+      <c r="I18" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="J18" s="25" t="s">
+        <v>21</v>
       </c>
       <c r="K18" s="34" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
       <c r="L18" s="5" t="s">
-        <v>4</v>
+        <v>297</v>
       </c>
       <c r="M18" s="19"/>
       <c r="N18" s="19"/>
@@ -13562,28 +13538,28 @@
     </row>
     <row r="19" spans="1:27">
       <c r="A19" s="3"/>
-      <c r="B19" s="41"/>
-      <c r="C19" s="41"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="42"/>
       <c r="D19" s="2" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E19" s="28"/>
       <c r="F19" s="28"/>
       <c r="G19" s="28"/>
       <c r="H19" s="26" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="I19" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="J19" s="25" t="s">
-        <v>27</v>
+        <v>20</v>
+      </c>
+      <c r="J19" s="26" t="s">
+        <v>21</v>
       </c>
       <c r="K19" s="34" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M19" s="19"/>
       <c r="N19" s="19"/>
@@ -13603,28 +13579,28 @@
     </row>
     <row r="20" spans="1:27">
       <c r="A20" s="3"/>
-      <c r="B20" s="41"/>
-      <c r="C20" s="41"/>
+      <c r="B20" s="42"/>
+      <c r="C20" s="42"/>
       <c r="D20" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E20" s="28"/>
       <c r="F20" s="28"/>
       <c r="G20" s="28"/>
       <c r="H20" s="26" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="I20" s="26" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="J20" s="25" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="K20" s="34" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="L20" s="5" t="s">
-        <v>6</v>
+        <v>298</v>
       </c>
       <c r="M20" s="19"/>
       <c r="N20" s="19"/>
@@ -13644,28 +13620,28 @@
     </row>
     <row r="21" spans="1:27">
       <c r="A21" s="3"/>
-      <c r="B21" s="41"/>
-      <c r="C21" s="41"/>
+      <c r="B21" s="42"/>
+      <c r="C21" s="42"/>
       <c r="D21" s="2" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E21" s="28"/>
       <c r="F21" s="28"/>
       <c r="G21" s="28"/>
       <c r="H21" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="I21" s="25" t="s">
-        <v>26</v>
+        <v>19</v>
+      </c>
+      <c r="I21" s="26" t="s">
+        <v>20</v>
       </c>
       <c r="J21" s="25" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="K21" s="34" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="L21" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="M21" s="19"/>
       <c r="N21" s="19"/>
@@ -13685,28 +13661,28 @@
     </row>
     <row r="22" spans="1:27">
       <c r="A22" s="3"/>
-      <c r="B22" s="41"/>
-      <c r="C22" s="41"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="42"/>
       <c r="D22" s="2" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="E22" s="28"/>
       <c r="F22" s="28"/>
       <c r="G22" s="28"/>
       <c r="H22" s="26" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="I22" s="25" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="J22" s="25" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="K22" s="34" t="s">
-        <v>294</v>
+        <v>258</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>8</v>
+        <v>300</v>
       </c>
       <c r="M22" s="19"/>
       <c r="N22" s="19"/>
@@ -13724,30 +13700,30 @@
       <c r="Z22" s="3"/>
       <c r="AA22" s="3"/>
     </row>
-    <row r="23" spans="1:27" ht="18" customHeight="1">
+    <row r="23" spans="1:27">
       <c r="A23" s="3"/>
-      <c r="B23" s="41"/>
-      <c r="C23" s="41"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="42"/>
       <c r="D23" s="2" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E23" s="28"/>
       <c r="F23" s="28"/>
       <c r="G23" s="28"/>
       <c r="H23" s="26" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="I23" s="25" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="J23" s="25" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="K23" s="34" t="s">
-        <v>266</v>
+        <v>287</v>
       </c>
       <c r="L23" s="5" t="s">
-        <v>9</v>
+        <v>301</v>
       </c>
       <c r="M23" s="19"/>
       <c r="N23" s="19"/>
@@ -13765,30 +13741,30 @@
       <c r="Z23" s="3"/>
       <c r="AA23" s="3"/>
     </row>
-    <row r="24" spans="1:27">
+    <row r="24" spans="1:27" ht="18" customHeight="1">
       <c r="A24" s="3"/>
-      <c r="B24" s="41"/>
-      <c r="C24" s="41"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="42"/>
       <c r="D24" s="2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E24" s="28"/>
       <c r="F24" s="28"/>
       <c r="G24" s="28"/>
       <c r="H24" s="26" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="I24" s="25" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="J24" s="25" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="K24" s="34" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>10</v>
+        <v>303</v>
       </c>
       <c r="M24" s="19"/>
       <c r="N24" s="19"/>
@@ -13808,28 +13784,28 @@
     </row>
     <row r="25" spans="1:27">
       <c r="A25" s="3"/>
-      <c r="B25" s="41"/>
-      <c r="C25" s="41"/>
+      <c r="B25" s="42"/>
+      <c r="C25" s="42"/>
       <c r="D25" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E25" s="28"/>
       <c r="F25" s="28"/>
       <c r="G25" s="28"/>
       <c r="H25" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="I25" s="26" t="s">
-        <v>26</v>
+        <v>19</v>
+      </c>
+      <c r="I25" s="25" t="s">
+        <v>20</v>
       </c>
       <c r="J25" s="25" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="K25" s="34" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="L25" s="5" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="M25" s="19"/>
       <c r="N25" s="19"/>
@@ -13849,28 +13825,28 @@
     </row>
     <row r="26" spans="1:27">
       <c r="A26" s="3"/>
-      <c r="B26" s="41"/>
-      <c r="C26" s="41"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="42"/>
       <c r="D26" s="2" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="E26" s="28"/>
       <c r="F26" s="28"/>
       <c r="G26" s="28"/>
       <c r="H26" s="26" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="I26" s="26" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="J26" s="25" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="K26" s="34" t="s">
-        <v>279</v>
+        <v>261</v>
       </c>
       <c r="L26" s="5" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="M26" s="19"/>
       <c r="N26" s="19"/>
@@ -13880,42 +13856,38 @@
       <c r="R26" s="3"/>
       <c r="S26" s="3"/>
       <c r="T26" s="3"/>
-      <c r="U26" s="38" t="s">
-        <v>127</v>
-      </c>
-      <c r="V26" s="38"/>
+      <c r="U26" s="3"/>
+      <c r="V26" s="3"/>
       <c r="W26" s="3"/>
       <c r="X26" s="3"/>
       <c r="Y26" s="3"/>
       <c r="Z26" s="3"/>
       <c r="AA26" s="3"/>
     </row>
-    <row r="27" spans="1:27" ht="18" customHeight="1">
+    <row r="27" spans="1:27">
       <c r="A27" s="3"/>
-      <c r="B27" s="39" t="s">
-        <v>47</v>
-      </c>
-      <c r="C27" s="39"/>
-      <c r="D27" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
       <c r="H27" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="I27" s="25" t="s">
-        <v>26</v>
+        <v>19</v>
+      </c>
+      <c r="I27" s="26" t="s">
+        <v>20</v>
       </c>
       <c r="J27" s="25" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="K27" s="34" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="L27" s="5" t="s">
-        <v>296</v>
+        <v>304</v>
       </c>
       <c r="M27" s="19"/>
       <c r="N27" s="19"/>
@@ -13925,38 +13897,42 @@
       <c r="R27" s="3"/>
       <c r="S27" s="3"/>
       <c r="T27" s="3"/>
-      <c r="U27" s="3"/>
-      <c r="V27" s="3"/>
+      <c r="U27" s="39" t="s">
+        <v>121</v>
+      </c>
+      <c r="V27" s="39"/>
       <c r="W27" s="3"/>
       <c r="X27" s="3"/>
       <c r="Y27" s="3"/>
       <c r="Z27" s="3"/>
       <c r="AA27" s="3"/>
     </row>
-    <row r="28" spans="1:27">
+    <row r="28" spans="1:27" ht="18" customHeight="1">
       <c r="A28" s="3"/>
-      <c r="B28" s="39"/>
-      <c r="C28" s="39"/>
+      <c r="B28" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" s="40"/>
       <c r="D28" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="E28" s="24"/>
       <c r="F28" s="24"/>
       <c r="G28" s="24"/>
       <c r="H28" s="26" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="I28" s="25" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="J28" s="25" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="K28" s="34" t="s">
-        <v>270</v>
-      </c>
-      <c r="L28" s="6" t="s">
-        <v>13</v>
+        <v>262</v>
+      </c>
+      <c r="L28" s="5" t="s">
+        <v>289</v>
       </c>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -13974,30 +13950,30 @@
       <c r="Z28" s="3"/>
       <c r="AA28" s="3"/>
     </row>
-    <row r="29" spans="1:27" ht="18" customHeight="1">
+    <row r="29" spans="1:27">
       <c r="A29" s="3"/>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
       <c r="D29" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E29" s="24"/>
       <c r="F29" s="24"/>
       <c r="G29" s="24"/>
       <c r="H29" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="I29" s="26" t="s">
-        <v>26</v>
+        <v>19</v>
+      </c>
+      <c r="I29" s="25" t="s">
+        <v>20</v>
       </c>
       <c r="J29" s="25" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="K29" s="34" t="s">
-        <v>271</v>
-      </c>
-      <c r="L29" s="5" t="s">
-        <v>14</v>
+        <v>263</v>
+      </c>
+      <c r="L29" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="M29" s="19"/>
       <c r="N29" s="19"/>
@@ -14015,30 +13991,30 @@
       <c r="Z29" s="3"/>
       <c r="AA29" s="3"/>
     </row>
-    <row r="30" spans="1:27">
+    <row r="30" spans="1:27" ht="18" customHeight="1">
       <c r="A30" s="3"/>
-      <c r="B30" s="39"/>
-      <c r="C30" s="39"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
       <c r="D30" s="1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="E30" s="24"/>
       <c r="F30" s="24"/>
       <c r="G30" s="24"/>
       <c r="H30" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="I30" s="25" t="s">
-        <v>26</v>
+        <v>19</v>
+      </c>
+      <c r="I30" s="26" t="s">
+        <v>20</v>
       </c>
       <c r="J30" s="25" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="K30" s="34" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="L30" s="5" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="M30" s="19"/>
       <c r="N30" s="19"/>
@@ -14058,37 +14034,35 @@
     </row>
     <row r="31" spans="1:27">
       <c r="A31" s="3"/>
-      <c r="B31" s="39"/>
-      <c r="C31" s="39"/>
+      <c r="B31" s="40"/>
+      <c r="C31" s="40"/>
       <c r="D31" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="E31" s="24"/>
       <c r="F31" s="24"/>
       <c r="G31" s="24"/>
       <c r="H31" s="26" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="I31" s="25" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="J31" s="25" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="K31" s="34" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="L31" s="5" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="M31" s="19"/>
       <c r="N31" s="19"/>
       <c r="O31" s="19"/>
       <c r="P31" s="3"/>
       <c r="Q31" s="3"/>
-      <c r="R31" s="5" t="s">
-        <v>53</v>
-      </c>
+      <c r="R31" s="3"/>
       <c r="S31" s="3"/>
       <c r="T31" s="3"/>
       <c r="U31" s="3"/>
@@ -14099,39 +14073,39 @@
       <c r="Z31" s="3"/>
       <c r="AA31" s="3"/>
     </row>
-    <row r="32" spans="1:27" ht="18" customHeight="1">
+    <row r="32" spans="1:27">
       <c r="A32" s="3"/>
-      <c r="B32" s="41" t="s">
-        <v>54</v>
-      </c>
-      <c r="C32" s="41"/>
-      <c r="D32" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="28"/>
+      <c r="B32" s="40"/>
+      <c r="C32" s="40"/>
+      <c r="D32" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="24"/>
       <c r="H32" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="I32" s="26" t="s">
-        <v>26</v>
+        <v>19</v>
+      </c>
+      <c r="I32" s="25" t="s">
+        <v>20</v>
       </c>
       <c r="J32" s="25" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="K32" s="34" t="s">
-        <v>274</v>
-      </c>
-      <c r="L32" s="36" t="s">
-        <v>297</v>
+        <v>266</v>
+      </c>
+      <c r="L32" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="M32" s="19"/>
       <c r="N32" s="19"/>
       <c r="O32" s="19"/>
       <c r="P32" s="3"/>
       <c r="Q32" s="3"/>
-      <c r="R32" s="3"/>
+      <c r="R32" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="S32" s="3"/>
       <c r="T32" s="3"/>
       <c r="U32" s="3"/>
@@ -14142,30 +14116,32 @@
       <c r="Z32" s="3"/>
       <c r="AA32" s="3"/>
     </row>
-    <row r="33" spans="1:27">
+    <row r="33" spans="1:27" ht="18" customHeight="1">
       <c r="A33" s="3"/>
-      <c r="B33" s="41"/>
-      <c r="C33" s="41"/>
+      <c r="B33" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="C33" s="42"/>
       <c r="D33" s="2" t="s">
-        <v>237</v>
+        <v>49</v>
       </c>
       <c r="E33" s="28"/>
       <c r="F33" s="28"/>
       <c r="G33" s="28"/>
       <c r="H33" s="26" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="I33" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="J33" s="26" t="s">
-        <v>27</v>
+        <v>20</v>
+      </c>
+      <c r="J33" s="25" t="s">
+        <v>21</v>
       </c>
       <c r="K33" s="34" t="s">
-        <v>275</v>
-      </c>
-      <c r="L33" s="19" t="s">
-        <v>241</v>
+        <v>267</v>
+      </c>
+      <c r="L33" s="36" t="s">
+        <v>290</v>
       </c>
       <c r="M33" s="19"/>
       <c r="N33" s="19"/>
@@ -14185,28 +14161,28 @@
     </row>
     <row r="34" spans="1:27">
       <c r="A34" s="3"/>
-      <c r="B34" s="41"/>
-      <c r="C34" s="41"/>
+      <c r="B34" s="42"/>
+      <c r="C34" s="42"/>
       <c r="D34" s="2" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="E34" s="28"/>
       <c r="F34" s="28"/>
       <c r="G34" s="28"/>
       <c r="H34" s="26" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="I34" s="26" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="J34" s="26" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="K34" s="34" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="L34" s="19" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="M34" s="19"/>
       <c r="N34" s="19"/>
@@ -14226,25 +14202,29 @@
     </row>
     <row r="35" spans="1:27">
       <c r="A35" s="3"/>
-      <c r="B35" s="41"/>
-      <c r="C35" s="41"/>
+      <c r="B35" s="42"/>
+      <c r="C35" s="42"/>
       <c r="D35" s="2" t="s">
-        <v>56</v>
+        <v>234</v>
       </c>
       <c r="E35" s="28"/>
       <c r="F35" s="28"/>
       <c r="G35" s="28"/>
       <c r="H35" s="26" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="I35" s="26" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="J35" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="K35" s="34"/>
-      <c r="L35" s="19"/>
+        <v>21</v>
+      </c>
+      <c r="K35" s="34" t="s">
+        <v>269</v>
+      </c>
+      <c r="L35" s="19" t="s">
+        <v>236</v>
+      </c>
       <c r="M35" s="19"/>
       <c r="N35" s="19"/>
       <c r="O35" s="19"/>
@@ -14263,29 +14243,25 @@
     </row>
     <row r="36" spans="1:27">
       <c r="A36" s="3"/>
-      <c r="B36" s="41"/>
-      <c r="C36" s="41"/>
+      <c r="B36" s="42"/>
+      <c r="C36" s="42"/>
       <c r="D36" s="2" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="E36" s="28"/>
       <c r="F36" s="28"/>
       <c r="G36" s="28"/>
-      <c r="H36" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="I36" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="J36" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="K36" s="34" t="s">
-        <v>277</v>
-      </c>
-      <c r="L36" s="19" t="s">
-        <v>243</v>
-      </c>
+      <c r="H36" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="I36" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="J36" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="K36" s="34"/>
+      <c r="L36" s="19"/>
       <c r="M36" s="19"/>
       <c r="N36" s="19"/>
       <c r="O36" s="19"/>
@@ -14302,30 +14278,30 @@
       <c r="Z36" s="3"/>
       <c r="AA36" s="3"/>
     </row>
-    <row r="37" spans="1:27" ht="17.399999999999999" customHeight="1">
+    <row r="37" spans="1:27">
       <c r="A37" s="3"/>
-      <c r="B37" s="41"/>
-      <c r="C37" s="41"/>
+      <c r="B37" s="42"/>
+      <c r="C37" s="42"/>
       <c r="D37" s="2" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="E37" s="28"/>
       <c r="F37" s="28"/>
       <c r="G37" s="28"/>
       <c r="H37" s="27" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="I37" s="27" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="J37" s="25" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="K37" s="34" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="L37" s="19" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="M37" s="19"/>
       <c r="N37" s="19"/>
@@ -14343,30 +14319,30 @@
       <c r="Z37" s="3"/>
       <c r="AA37" s="3"/>
     </row>
-    <row r="38" spans="1:27">
+    <row r="38" spans="1:27" ht="17.399999999999999" customHeight="1">
       <c r="A38" s="3"/>
-      <c r="B38" s="41"/>
-      <c r="C38" s="41"/>
+      <c r="B38" s="42"/>
+      <c r="C38" s="42"/>
       <c r="D38" s="2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="E38" s="28"/>
       <c r="F38" s="28"/>
       <c r="G38" s="28"/>
-      <c r="H38" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="I38" s="26" t="s">
-        <v>26</v>
+      <c r="H38" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="I38" s="27" t="s">
+        <v>20</v>
       </c>
       <c r="J38" s="25" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="K38" s="34" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="L38" s="19" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="M38" s="19"/>
       <c r="N38" s="19"/>
@@ -14384,27 +14360,31 @@
       <c r="Z38" s="3"/>
       <c r="AA38" s="3"/>
     </row>
-    <row r="39" spans="1:27">
+    <row r="39" spans="1:27" ht="409.6">
       <c r="A39" s="3"/>
-      <c r="B39" s="41"/>
-      <c r="C39" s="41"/>
+      <c r="B39" s="42"/>
+      <c r="C39" s="42"/>
       <c r="D39" s="2" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E39" s="28"/>
       <c r="F39" s="28"/>
       <c r="G39" s="28"/>
       <c r="H39" s="26" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="I39" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="J39" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="K39" s="34"/>
-      <c r="L39" s="19"/>
+        <v>20</v>
+      </c>
+      <c r="J39" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="K39" s="34" t="s">
+        <v>273</v>
+      </c>
+      <c r="L39" s="19" t="s">
+        <v>239</v>
+      </c>
       <c r="M39" s="19"/>
       <c r="N39" s="19"/>
       <c r="O39" s="19"/>
@@ -14421,33 +14401,27 @@
       <c r="Z39" s="3"/>
       <c r="AA39" s="3"/>
     </row>
-    <row r="40" spans="1:27" ht="18" customHeight="1">
+    <row r="40" spans="1:27">
       <c r="A40" s="3"/>
-      <c r="B40" s="39" t="s">
-        <v>61</v>
-      </c>
-      <c r="C40" s="39"/>
-      <c r="D40" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E40" s="24"/>
-      <c r="F40" s="24"/>
-      <c r="G40" s="24"/>
+      <c r="B40" s="42"/>
+      <c r="C40" s="42"/>
+      <c r="D40" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E40" s="28"/>
+      <c r="F40" s="28"/>
+      <c r="G40" s="28"/>
       <c r="H40" s="26" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="I40" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="J40" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="K40" s="34" t="s">
-        <v>251</v>
-      </c>
-      <c r="L40" s="19" t="s">
-        <v>222</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="J40" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="K40" s="34"/>
+      <c r="L40" s="19"/>
       <c r="M40" s="19"/>
       <c r="N40" s="19"/>
       <c r="O40" s="19"/>
@@ -14466,28 +14440,30 @@
     </row>
     <row r="41" spans="1:27" ht="18" customHeight="1">
       <c r="A41" s="3"/>
-      <c r="B41" s="39"/>
-      <c r="C41" s="39"/>
+      <c r="B41" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="C41" s="40"/>
       <c r="D41" s="1" t="s">
-        <v>219</v>
+        <v>56</v>
       </c>
       <c r="E41" s="24"/>
       <c r="F41" s="24"/>
       <c r="G41" s="24"/>
       <c r="H41" s="26" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="I41" s="26" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="J41" s="25" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="K41" s="34" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="L41" s="19" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="M41" s="19"/>
       <c r="N41" s="19"/>
@@ -14505,30 +14481,30 @@
       <c r="Z41" s="3"/>
       <c r="AA41" s="3"/>
     </row>
-    <row r="42" spans="1:27">
+    <row r="42" spans="1:27" ht="18" customHeight="1">
       <c r="A42" s="3"/>
-      <c r="B42" s="39"/>
-      <c r="C42" s="39"/>
+      <c r="B42" s="40"/>
+      <c r="C42" s="40"/>
       <c r="D42" s="1" t="s">
-        <v>238</v>
+        <v>213</v>
       </c>
       <c r="E42" s="24"/>
       <c r="F42" s="24"/>
       <c r="G42" s="24"/>
       <c r="H42" s="26" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="I42" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="J42" s="26" t="s">
-        <v>27</v>
+        <v>20</v>
+      </c>
+      <c r="J42" s="25" t="s">
+        <v>21</v>
       </c>
       <c r="K42" s="34" t="s">
-        <v>281</v>
+        <v>245</v>
       </c>
       <c r="L42" s="19" t="s">
-        <v>239</v>
+        <v>214</v>
       </c>
       <c r="M42" s="19"/>
       <c r="N42" s="19"/>
@@ -14548,28 +14524,28 @@
     </row>
     <row r="43" spans="1:27">
       <c r="A43" s="3"/>
-      <c r="B43" s="39"/>
-      <c r="C43" s="39"/>
+      <c r="B43" s="40"/>
+      <c r="C43" s="40"/>
       <c r="D43" s="1" t="s">
-        <v>221</v>
+        <v>232</v>
       </c>
       <c r="E43" s="24"/>
       <c r="F43" s="24"/>
       <c r="G43" s="24"/>
       <c r="H43" s="26" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="I43" s="26" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="J43" s="26" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="K43" s="34" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="L43" s="19" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="M43" s="19"/>
       <c r="N43" s="19"/>
@@ -14589,25 +14565,25 @@
     </row>
     <row r="44" spans="1:27">
       <c r="A44" s="3"/>
-      <c r="B44" s="39"/>
-      <c r="C44" s="39"/>
+      <c r="B44" s="40"/>
+      <c r="C44" s="40"/>
       <c r="D44" s="1" t="s">
-        <v>63</v>
+        <v>215</v>
       </c>
       <c r="E44" s="24"/>
       <c r="F44" s="24"/>
       <c r="G44" s="24"/>
       <c r="H44" s="26" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="I44" s="26" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="J44" s="26" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="K44" s="34" t="s">
-        <v>253</v>
+        <v>275</v>
       </c>
       <c r="L44" s="19" t="s">
         <v>223</v>
@@ -14630,28 +14606,28 @@
     </row>
     <row r="45" spans="1:27">
       <c r="A45" s="3"/>
-      <c r="B45" s="39"/>
-      <c r="C45" s="39"/>
+      <c r="B45" s="40"/>
+      <c r="C45" s="40"/>
       <c r="D45" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E45" s="24"/>
       <c r="F45" s="24"/>
       <c r="G45" s="24"/>
       <c r="H45" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="I45" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="J45" s="25" t="s">
-        <v>27</v>
+        <v>19</v>
+      </c>
+      <c r="I45" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="J45" s="26" t="s">
+        <v>21</v>
       </c>
       <c r="K45" s="34" t="s">
-        <v>283</v>
+        <v>246</v>
       </c>
       <c r="L45" s="19" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="M45" s="19"/>
       <c r="N45" s="19"/>
@@ -14671,28 +14647,28 @@
     </row>
     <row r="46" spans="1:27">
       <c r="A46" s="3"/>
-      <c r="B46" s="39"/>
-      <c r="C46" s="39"/>
+      <c r="B46" s="40"/>
+      <c r="C46" s="40"/>
       <c r="D46" s="1" t="s">
-        <v>224</v>
+        <v>58</v>
       </c>
       <c r="E46" s="24"/>
       <c r="F46" s="24"/>
       <c r="G46" s="24"/>
       <c r="H46" s="26" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="I46" s="27" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="J46" s="25" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="K46" s="34" t="s">
-        <v>254</v>
+        <v>276</v>
       </c>
       <c r="L46" s="19" t="s">
-        <v>298</v>
+        <v>219</v>
       </c>
       <c r="M46" s="19"/>
       <c r="N46" s="19"/>
@@ -14712,28 +14688,28 @@
     </row>
     <row r="47" spans="1:27">
       <c r="A47" s="3"/>
-      <c r="B47" s="39"/>
-      <c r="C47" s="39"/>
+      <c r="B47" s="40"/>
+      <c r="C47" s="40"/>
       <c r="D47" s="1" t="s">
-        <v>65</v>
+        <v>218</v>
       </c>
       <c r="E47" s="24"/>
       <c r="F47" s="24"/>
       <c r="G47" s="24"/>
       <c r="H47" s="26" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="I47" s="27" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="J47" s="25" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="K47" s="34" t="s">
-        <v>284</v>
+        <v>247</v>
       </c>
       <c r="L47" s="19" t="s">
-        <v>226</v>
+        <v>291</v>
       </c>
       <c r="M47" s="19"/>
       <c r="N47" s="19"/>
@@ -14753,28 +14729,28 @@
     </row>
     <row r="48" spans="1:27">
       <c r="A48" s="3"/>
-      <c r="B48" s="39"/>
-      <c r="C48" s="39"/>
+      <c r="B48" s="40"/>
+      <c r="C48" s="40"/>
       <c r="D48" s="1" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E48" s="24"/>
       <c r="F48" s="24"/>
       <c r="G48" s="24"/>
       <c r="H48" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="I48" s="26" t="s">
-        <v>26</v>
+        <v>19</v>
+      </c>
+      <c r="I48" s="27" t="s">
+        <v>20</v>
       </c>
       <c r="J48" s="25" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="K48" s="34" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="L48" s="19" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="M48" s="19"/>
       <c r="N48" s="19"/>
@@ -14792,32 +14768,30 @@
       <c r="Z48" s="3"/>
       <c r="AA48" s="3"/>
     </row>
-    <row r="49" spans="1:27" ht="18" customHeight="1">
+    <row r="49" spans="1:27">
       <c r="A49" s="3"/>
-      <c r="B49" s="41" t="s">
-        <v>67</v>
-      </c>
-      <c r="C49" s="41"/>
-      <c r="D49" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E49" s="28"/>
-      <c r="F49" s="28"/>
-      <c r="G49" s="28"/>
+      <c r="B49" s="40"/>
+      <c r="C49" s="40"/>
+      <c r="D49" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E49" s="24"/>
+      <c r="F49" s="24"/>
+      <c r="G49" s="24"/>
       <c r="H49" s="26" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="I49" s="26" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="J49" s="25" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="K49" s="34" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="L49" s="19" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="M49" s="19"/>
       <c r="N49" s="19"/>
@@ -14835,30 +14809,32 @@
       <c r="Z49" s="3"/>
       <c r="AA49" s="3"/>
     </row>
-    <row r="50" spans="1:27">
+    <row r="50" spans="1:27" ht="18" customHeight="1">
       <c r="A50" s="3"/>
-      <c r="B50" s="41"/>
-      <c r="C50" s="41"/>
+      <c r="B50" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="C50" s="42"/>
       <c r="D50" s="2" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="E50" s="28"/>
       <c r="F50" s="28"/>
       <c r="G50" s="28"/>
       <c r="H50" s="26" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="I50" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="J50" s="26" t="s">
-        <v>27</v>
+        <v>20</v>
+      </c>
+      <c r="J50" s="25" t="s">
+        <v>21</v>
       </c>
       <c r="K50" s="34" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="L50" s="19" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="M50" s="19"/>
       <c r="N50" s="19"/>
@@ -14878,28 +14854,28 @@
     </row>
     <row r="51" spans="1:27">
       <c r="A51" s="3"/>
-      <c r="B51" s="41"/>
-      <c r="C51" s="41"/>
+      <c r="B51" s="42"/>
+      <c r="C51" s="42"/>
       <c r="D51" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="E51" s="28"/>
       <c r="F51" s="28"/>
       <c r="G51" s="28"/>
       <c r="H51" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="I51" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="J51" s="25" t="s">
-        <v>27</v>
+        <v>19</v>
+      </c>
+      <c r="I51" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="J51" s="26" t="s">
+        <v>21</v>
       </c>
       <c r="K51" s="34" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="L51" s="19" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="M51" s="19"/>
       <c r="N51" s="19"/>
@@ -14919,28 +14895,28 @@
     </row>
     <row r="52" spans="1:27">
       <c r="A52" s="3"/>
-      <c r="B52" s="41"/>
-      <c r="C52" s="41"/>
+      <c r="B52" s="42"/>
+      <c r="C52" s="42"/>
       <c r="D52" s="2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="E52" s="28"/>
       <c r="F52" s="28"/>
       <c r="G52" s="28"/>
       <c r="H52" s="26" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="I52" s="27" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="J52" s="25" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="K52" s="34" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="L52" s="19" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="M52" s="19"/>
       <c r="N52" s="19"/>
@@ -14958,32 +14934,30 @@
       <c r="Z52" s="3"/>
       <c r="AA52" s="3"/>
     </row>
-    <row r="53" spans="1:27" ht="18" customHeight="1">
+    <row r="53" spans="1:27">
       <c r="A53" s="3"/>
-      <c r="B53" s="39" t="s">
-        <v>72</v>
-      </c>
-      <c r="C53" s="39"/>
-      <c r="D53" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E53" s="24"/>
-      <c r="F53" s="24"/>
-      <c r="G53" s="24"/>
+      <c r="B53" s="42"/>
+      <c r="C53" s="42"/>
+      <c r="D53" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E53" s="28"/>
+      <c r="F53" s="28"/>
+      <c r="G53" s="28"/>
       <c r="H53" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="I53" s="26" t="s">
-        <v>26</v>
+        <v>19</v>
+      </c>
+      <c r="I53" s="27" t="s">
+        <v>20</v>
       </c>
       <c r="J53" s="25" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="K53" s="34" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="L53" s="19" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="M53" s="19"/>
       <c r="N53" s="19"/>
@@ -15001,30 +14975,32 @@
       <c r="Z53" s="3"/>
       <c r="AA53" s="3"/>
     </row>
-    <row r="54" spans="1:27">
+    <row r="54" spans="1:27" ht="18" customHeight="1">
       <c r="A54" s="3"/>
-      <c r="B54" s="39"/>
-      <c r="C54" s="39"/>
+      <c r="B54" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="C54" s="40"/>
       <c r="D54" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="E54" s="24"/>
       <c r="F54" s="24"/>
       <c r="G54" s="24"/>
       <c r="H54" s="26" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="I54" s="26" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="J54" s="25" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="K54" s="34" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="L54" s="19" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="M54" s="19"/>
       <c r="N54" s="19"/>
@@ -15044,25 +15020,29 @@
     </row>
     <row r="55" spans="1:27">
       <c r="A55" s="3"/>
-      <c r="B55" s="39"/>
-      <c r="C55" s="39"/>
+      <c r="B55" s="40"/>
+      <c r="C55" s="40"/>
       <c r="D55" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E55" s="24"/>
       <c r="F55" s="24"/>
       <c r="G55" s="24"/>
       <c r="H55" s="26" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="I55" s="26" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="J55" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="K55" s="34"/>
-      <c r="L55" s="19"/>
+        <v>21</v>
+      </c>
+      <c r="K55" s="34" t="s">
+        <v>284</v>
+      </c>
+      <c r="L55" s="19" t="s">
+        <v>228</v>
+      </c>
       <c r="M55" s="19"/>
       <c r="N55" s="19"/>
       <c r="O55" s="19"/>
@@ -15081,29 +15061,25 @@
     </row>
     <row r="56" spans="1:27">
       <c r="A56" s="3"/>
-      <c r="B56" s="39"/>
-      <c r="C56" s="39"/>
+      <c r="B56" s="40"/>
+      <c r="C56" s="40"/>
       <c r="D56" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="E56" s="24"/>
       <c r="F56" s="24"/>
       <c r="G56" s="24"/>
       <c r="H56" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="I56" s="27" t="s">
-        <v>26</v>
+        <v>19</v>
+      </c>
+      <c r="I56" s="26" t="s">
+        <v>20</v>
       </c>
       <c r="J56" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="K56" s="34" t="s">
-        <v>292</v>
-      </c>
-      <c r="L56" s="19" t="s">
-        <v>235</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="K56" s="34"/>
+      <c r="L56" s="19"/>
       <c r="M56" s="19"/>
       <c r="N56" s="19"/>
       <c r="O56" s="19"/>
@@ -15122,28 +15098,28 @@
     </row>
     <row r="57" spans="1:27">
       <c r="A57" s="3"/>
-      <c r="B57" s="39"/>
-      <c r="C57" s="39"/>
+      <c r="B57" s="40"/>
+      <c r="C57" s="40"/>
       <c r="D57" s="1" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="E57" s="24"/>
       <c r="F57" s="24"/>
       <c r="G57" s="24"/>
       <c r="H57" s="26" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="I57" s="27" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="J57" s="25" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="K57" s="34" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="L57" s="19" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="M57" s="19"/>
       <c r="N57" s="19"/>
@@ -15163,20 +15139,32 @@
     </row>
     <row r="58" spans="1:27">
       <c r="A58" s="3"/>
-      <c r="B58" s="3"/>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
-      <c r="E58" s="3"/>
-      <c r="F58" s="3"/>
-      <c r="G58" s="3"/>
-      <c r="H58" s="3"/>
-      <c r="I58" s="3"/>
-      <c r="J58" s="3"/>
-      <c r="K58" s="31"/>
-      <c r="L58" s="3"/>
-      <c r="M58" s="3"/>
-      <c r="N58" s="3"/>
-      <c r="O58" s="3"/>
+      <c r="B58" s="40"/>
+      <c r="C58" s="40"/>
+      <c r="D58" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E58" s="24"/>
+      <c r="F58" s="24"/>
+      <c r="G58" s="24"/>
+      <c r="H58" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="I58" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="J58" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="K58" s="34" t="s">
+        <v>286</v>
+      </c>
+      <c r="L58" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="M58" s="19"/>
+      <c r="N58" s="19"/>
+      <c r="O58" s="19"/>
       <c r="P58" s="3"/>
       <c r="Q58" s="3"/>
       <c r="R58" s="3"/>
@@ -15248,15 +15236,13 @@
       <c r="Z60" s="3"/>
       <c r="AA60" s="3"/>
     </row>
-    <row r="61" spans="1:27" ht="18" customHeight="1">
+    <row r="61" spans="1:27">
       <c r="A61" s="3"/>
-      <c r="B61" s="37" t="s">
-        <v>78</v>
-      </c>
-      <c r="C61" s="37"/>
-      <c r="D61" s="37"/>
-      <c r="E61" s="37"/>
-      <c r="F61" s="37"/>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3"/>
       <c r="G61" s="3"/>
       <c r="H61" s="3"/>
       <c r="I61" s="3"/>
@@ -15279,13 +15265,15 @@
       <c r="Z61" s="3"/>
       <c r="AA61" s="3"/>
     </row>
-    <row r="62" spans="1:27">
+    <row r="62" spans="1:27" ht="18" customHeight="1">
       <c r="A62" s="3"/>
-      <c r="B62" s="37"/>
-      <c r="C62" s="37"/>
-      <c r="D62" s="37"/>
-      <c r="E62" s="37"/>
-      <c r="F62" s="37"/>
+      <c r="B62" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="C62" s="38"/>
+      <c r="D62" s="38"/>
+      <c r="E62" s="38"/>
+      <c r="F62" s="38"/>
       <c r="G62" s="3"/>
       <c r="H62" s="3"/>
       <c r="I62" s="3"/>
@@ -15308,17 +15296,13 @@
       <c r="Z62" s="3"/>
       <c r="AA62" s="3"/>
     </row>
-    <row r="63" spans="1:27" ht="34">
+    <row r="63" spans="1:27">
       <c r="A63" s="3"/>
-      <c r="B63" s="7">
-        <v>1</v>
-      </c>
-      <c r="C63" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="D63" s="3"/>
-      <c r="E63" s="3"/>
-      <c r="F63" s="3"/>
+      <c r="B63" s="38"/>
+      <c r="C63" s="38"/>
+      <c r="D63" s="38"/>
+      <c r="E63" s="38"/>
+      <c r="F63" s="38"/>
       <c r="G63" s="3"/>
       <c r="H63" s="3"/>
       <c r="I63" s="3"/>
@@ -15344,10 +15328,10 @@
     <row r="64" spans="1:27" ht="34">
       <c r="A64" s="3"/>
       <c r="B64" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C64" s="29" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
@@ -15376,15 +15360,15 @@
     </row>
     <row r="65" spans="1:27" ht="34">
       <c r="A65" s="3"/>
-      <c r="B65" s="8">
-        <v>3</v>
-      </c>
-      <c r="C65" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="D65" s="9"/>
-      <c r="E65" s="9"/>
-      <c r="F65" s="9"/>
+      <c r="B65" s="7">
+        <v>2</v>
+      </c>
+      <c r="C65" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="D65" s="3"/>
+      <c r="E65" s="3"/>
+      <c r="F65" s="3"/>
       <c r="G65" s="3"/>
       <c r="H65" s="3"/>
       <c r="I65" s="3"/>
@@ -15407,10 +15391,14 @@
       <c r="Z65" s="3"/>
       <c r="AA65" s="3"/>
     </row>
-    <row r="66" spans="1:27">
+    <row r="66" spans="1:27" ht="34">
       <c r="A66" s="3"/>
-      <c r="B66" s="9"/>
-      <c r="C66" s="9"/>
+      <c r="B66" s="8">
+        <v>3</v>
+      </c>
+      <c r="C66" s="9" t="s">
+        <v>75</v>
+      </c>
       <c r="D66" s="9"/>
       <c r="E66" s="9"/>
       <c r="F66" s="9"/>
@@ -15438,11 +15426,11 @@
     </row>
     <row r="67" spans="1:27">
       <c r="A67" s="3"/>
-      <c r="B67" s="3"/>
-      <c r="C67" s="3"/>
-      <c r="D67" s="3"/>
-      <c r="E67" s="3"/>
-      <c r="F67" s="3"/>
+      <c r="B67" s="9"/>
+      <c r="C67" s="9"/>
+      <c r="D67" s="9"/>
+      <c r="E67" s="9"/>
+      <c r="F67" s="9"/>
       <c r="G67" s="3"/>
       <c r="H67" s="3"/>
       <c r="I67" s="3"/>
@@ -16626,33 +16614,33 @@
       <c r="AA107" s="3"/>
     </row>
     <row r="108" spans="1:27">
-      <c r="A108" s="10"/>
-      <c r="B108" s="10"/>
-      <c r="C108" s="10"/>
-      <c r="D108" s="10"/>
-      <c r="E108" s="10"/>
-      <c r="F108" s="10"/>
-      <c r="G108" s="10"/>
-      <c r="H108" s="10"/>
-      <c r="I108" s="10"/>
-      <c r="J108" s="10"/>
+      <c r="A108" s="3"/>
+      <c r="B108" s="3"/>
+      <c r="C108" s="3"/>
+      <c r="D108" s="3"/>
+      <c r="E108" s="3"/>
+      <c r="F108" s="3"/>
+      <c r="G108" s="3"/>
+      <c r="H108" s="3"/>
+      <c r="I108" s="3"/>
+      <c r="J108" s="3"/>
       <c r="K108" s="31"/>
-      <c r="L108" s="10"/>
-      <c r="M108" s="10"/>
-      <c r="N108" s="10"/>
-      <c r="O108" s="10"/>
-      <c r="P108" s="10"/>
-      <c r="Q108" s="10"/>
-      <c r="R108" s="10"/>
-      <c r="S108" s="10"/>
-      <c r="T108" s="10"/>
-      <c r="U108" s="10"/>
-      <c r="V108" s="10"/>
-      <c r="W108" s="10"/>
-      <c r="X108" s="10"/>
-      <c r="Y108" s="10"/>
-      <c r="Z108" s="10"/>
-      <c r="AA108" s="10"/>
+      <c r="L108" s="3"/>
+      <c r="M108" s="3"/>
+      <c r="N108" s="3"/>
+      <c r="O108" s="3"/>
+      <c r="P108" s="3"/>
+      <c r="Q108" s="3"/>
+      <c r="R108" s="3"/>
+      <c r="S108" s="3"/>
+      <c r="T108" s="3"/>
+      <c r="U108" s="3"/>
+      <c r="V108" s="3"/>
+      <c r="W108" s="3"/>
+      <c r="X108" s="3"/>
+      <c r="Y108" s="3"/>
+      <c r="Z108" s="3"/>
+      <c r="AA108" s="3"/>
     </row>
     <row r="109" spans="1:27">
       <c r="A109" s="10"/>
@@ -42870,18 +42858,47 @@
       <c r="Z1012" s="10"/>
       <c r="AA1012" s="10"/>
     </row>
+    <row r="1013" spans="1:27">
+      <c r="A1013" s="10"/>
+      <c r="B1013" s="10"/>
+      <c r="C1013" s="10"/>
+      <c r="D1013" s="10"/>
+      <c r="E1013" s="10"/>
+      <c r="F1013" s="10"/>
+      <c r="G1013" s="10"/>
+      <c r="H1013" s="10"/>
+      <c r="I1013" s="10"/>
+      <c r="J1013" s="10"/>
+      <c r="K1013" s="31"/>
+      <c r="L1013" s="10"/>
+      <c r="M1013" s="10"/>
+      <c r="N1013" s="10"/>
+      <c r="O1013" s="10"/>
+      <c r="P1013" s="10"/>
+      <c r="Q1013" s="10"/>
+      <c r="R1013" s="10"/>
+      <c r="S1013" s="10"/>
+      <c r="T1013" s="10"/>
+      <c r="U1013" s="10"/>
+      <c r="V1013" s="10"/>
+      <c r="W1013" s="10"/>
+      <c r="X1013" s="10"/>
+      <c r="Y1013" s="10"/>
+      <c r="Z1013" s="10"/>
+      <c r="AA1013" s="10"/>
+    </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="B61:F62"/>
-    <mergeCell ref="U26:V26"/>
-    <mergeCell ref="B8:C15"/>
-    <mergeCell ref="B5:J7"/>
-    <mergeCell ref="B16:C26"/>
-    <mergeCell ref="B27:C31"/>
-    <mergeCell ref="B32:C39"/>
-    <mergeCell ref="B40:C48"/>
-    <mergeCell ref="B49:C52"/>
-    <mergeCell ref="B53:C57"/>
+    <mergeCell ref="B62:F63"/>
+    <mergeCell ref="U27:V27"/>
+    <mergeCell ref="B9:C16"/>
+    <mergeCell ref="B6:J8"/>
+    <mergeCell ref="B17:C27"/>
+    <mergeCell ref="B28:C32"/>
+    <mergeCell ref="B33:C40"/>
+    <mergeCell ref="B41:C49"/>
+    <mergeCell ref="B50:C53"/>
+    <mergeCell ref="B54:C58"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -42906,676 +42923,642 @@
   <sheetData>
     <row r="5" spans="4:6" ht="17.5" thickBot="1">
       <c r="D5" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="4:6" ht="26" thickTop="1">
+      <c r="D6" s="43">
+        <v>1</v>
+      </c>
+      <c r="E6" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="4:6">
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="4:6" ht="26">
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="4:6" ht="25.5">
+      <c r="D9" s="43">
+        <v>2</v>
+      </c>
+      <c r="E9" s="43" t="s">
+        <v>81</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="4:6">
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="4:6">
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="E5" s="14" t="s">
+    </row>
+    <row r="12" spans="4:6">
+      <c r="D12" s="43">
+        <v>3</v>
+      </c>
+      <c r="E12" s="43" t="s">
+        <v>130</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="13" spans="4:6">
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="4:6">
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="4:6" ht="25">
+      <c r="D15" s="43">
+        <v>4</v>
+      </c>
+      <c r="E15" s="43" t="s">
+        <v>131</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="16" spans="4:6" ht="26">
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="4:6">
+      <c r="D17" s="44"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="4:6" ht="38">
+      <c r="D18" s="43">
+        <v>5</v>
+      </c>
+      <c r="E18" s="43" t="s">
+        <v>132</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="19" spans="4:6">
+      <c r="D19" s="44"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="4:6">
+      <c r="D20" s="44"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="21" spans="4:6">
+      <c r="D21" s="43">
+        <v>6</v>
+      </c>
+      <c r="E21" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="22" spans="4:6">
+      <c r="D22" s="44"/>
+      <c r="E22" s="44"/>
+      <c r="F22" s="12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="4:6">
+      <c r="D23" s="44"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="24" spans="4:6" ht="38">
+      <c r="D24" s="43">
+        <v>7</v>
+      </c>
+      <c r="E24" s="43" t="s">
+        <v>131</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="25" spans="4:6">
+      <c r="D25" s="44"/>
+      <c r="E25" s="44"/>
+      <c r="F25" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="4:6">
+      <c r="D26" s="44"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="4:6" ht="26">
+      <c r="D27" s="43">
+        <v>8</v>
+      </c>
+      <c r="E27" s="43" t="s">
+        <v>133</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="28" spans="4:6" ht="26">
+      <c r="D28" s="44"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="4:6">
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="30" spans="4:6" ht="25">
+      <c r="D30" s="43">
+        <v>9</v>
+      </c>
+      <c r="E30" s="43" t="s">
+        <v>81</v>
+      </c>
+      <c r="F30" s="13" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="31" spans="4:6">
+      <c r="D31" s="44"/>
+      <c r="E31" s="44"/>
+      <c r="F31" s="12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="32" spans="4:6">
+      <c r="D32" s="44"/>
+      <c r="E32" s="44"/>
+      <c r="F32" s="12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="4:6">
+      <c r="D33" s="43">
+        <v>10</v>
+      </c>
+      <c r="E33" s="43" t="s">
+        <v>81</v>
+      </c>
+      <c r="F33" s="13" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="34" spans="4:6">
+      <c r="D34" s="44"/>
+      <c r="E34" s="44"/>
+      <c r="F34" s="12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="35" spans="4:6">
+      <c r="D35" s="44"/>
+      <c r="E35" s="44"/>
+      <c r="F35" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="36" spans="4:6" ht="25">
+      <c r="D36" s="43">
+        <v>11</v>
+      </c>
+      <c r="E36" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="F36" s="13" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="37" spans="4:6">
+      <c r="D37" s="44"/>
+      <c r="E37" s="44"/>
+      <c r="F37" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="38" spans="4:6">
+      <c r="D38" s="44"/>
+      <c r="E38" s="44"/>
+      <c r="F38" s="12" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="39" spans="4:6" ht="37.5">
+      <c r="D39" s="43">
+        <v>12</v>
+      </c>
+      <c r="E39" s="43" t="s">
+        <v>135</v>
+      </c>
+      <c r="F39" s="13" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="40" spans="4:6">
+      <c r="D40" s="44"/>
+      <c r="E40" s="44"/>
+      <c r="F40" s="12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="41" spans="4:6">
+      <c r="D41" s="44"/>
+      <c r="E41" s="44"/>
+      <c r="F41" s="12" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="42" spans="4:6" ht="25">
+      <c r="D42" s="43">
+        <v>13</v>
+      </c>
+      <c r="E42" s="43" t="s">
+        <v>131</v>
+      </c>
+      <c r="F42" s="13" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="43" spans="4:6">
+      <c r="D43" s="44"/>
+      <c r="E43" s="44"/>
+      <c r="F43" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="44" spans="4:6">
+      <c r="D44" s="44"/>
+      <c r="E44" s="44"/>
+      <c r="F44" s="12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="45" spans="4:6" ht="75.5">
+      <c r="D45" s="43">
+        <v>14</v>
+      </c>
+      <c r="E45" s="43" t="s">
+        <v>136</v>
+      </c>
+      <c r="F45" s="13" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="46" spans="4:6" ht="26">
+      <c r="D46" s="44"/>
+      <c r="E46" s="44"/>
+      <c r="F46" s="12" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="47" spans="4:6">
+      <c r="D47" s="44"/>
+      <c r="E47" s="44"/>
+      <c r="F47" s="12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="48" spans="4:6" ht="37.5">
+      <c r="D48" s="43">
+        <v>15</v>
+      </c>
+      <c r="E48" s="43" t="s">
+        <v>137</v>
+      </c>
+      <c r="F48" s="13" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="49" spans="4:6" ht="26">
+      <c r="D49" s="44"/>
+      <c r="E49" s="44"/>
+      <c r="F49" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="50" spans="4:6">
+      <c r="D50" s="44"/>
+      <c r="E50" s="44"/>
+      <c r="F50" s="12" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="51" spans="4:6" ht="25">
+      <c r="D51" s="43">
+        <v>16</v>
+      </c>
+      <c r="E51" s="43" t="s">
+        <v>138</v>
+      </c>
+      <c r="F51" s="13" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="52" spans="4:6">
+      <c r="D52" s="44"/>
+      <c r="E52" s="44"/>
+      <c r="F52" s="12" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="53" spans="4:6">
+      <c r="D53" s="44"/>
+      <c r="E53" s="44"/>
+      <c r="F53" s="12" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="54" spans="4:6" ht="25">
+      <c r="D54" s="43">
+        <v>17</v>
+      </c>
+      <c r="E54" s="43" t="s">
+        <v>138</v>
+      </c>
+      <c r="F54" s="13" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="55" spans="4:6">
+      <c r="D55" s="44"/>
+      <c r="E55" s="44"/>
+      <c r="F55" s="12" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="56" spans="4:6">
+      <c r="D56" s="44"/>
+      <c r="E56" s="44"/>
+      <c r="F56" s="12" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="57" spans="4:6">
+      <c r="D57" s="43">
+        <v>18</v>
+      </c>
+      <c r="E57" s="43" t="s">
+        <v>81</v>
+      </c>
+      <c r="F57" s="13" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="58" spans="4:6">
+      <c r="D58" s="44"/>
+      <c r="E58" s="44"/>
+      <c r="F58" s="12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="59" spans="4:6">
+      <c r="D59" s="44"/>
+      <c r="E59" s="44"/>
+      <c r="F59" s="12" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="60" spans="4:6" ht="34">
+      <c r="D60" s="43">
+        <v>19</v>
+      </c>
+      <c r="E60" s="43" t="s">
+        <v>81</v>
+      </c>
+      <c r="F60" s="16" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="61" spans="4:6">
+      <c r="D61" s="44"/>
+      <c r="E61" s="44"/>
+      <c r="F61" s="12" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="62" spans="4:6">
+      <c r="D62" s="44"/>
+      <c r="E62" s="44"/>
+      <c r="F62" s="12" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="63" spans="4:6" ht="34">
+      <c r="D63" s="43">
+        <v>20</v>
+      </c>
+      <c r="E63" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="F5" s="14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="4:6" ht="26" thickTop="1">
-      <c r="D6" s="42">
-        <v>1</v>
-      </c>
-      <c r="E6" s="42" t="s">
-        <v>85</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="7" spans="4:6">
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="12" t="s">
+      <c r="F63" s="16" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="64" spans="4:6">
+      <c r="D64" s="44"/>
+      <c r="E64" s="44"/>
+      <c r="F64" s="12" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="65" spans="4:6">
+      <c r="D65" s="44"/>
+      <c r="E65" s="44"/>
+      <c r="F65" s="12" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="66" spans="4:6" ht="34">
+      <c r="D66" s="43">
+        <v>21</v>
+      </c>
+      <c r="E66" s="43" t="s">
+        <v>83</v>
+      </c>
+      <c r="F66" s="16" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="67" spans="4:6" ht="26">
+      <c r="D67" s="44"/>
+      <c r="E67" s="44"/>
+      <c r="F67" s="12" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="68" spans="4:6">
+      <c r="D68" s="44"/>
+      <c r="E68" s="44"/>
+      <c r="F68" s="12" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="69" spans="4:6" ht="34">
+      <c r="D69" s="43">
+        <v>22</v>
+      </c>
+      <c r="E69" s="43" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="8" spans="4:6" ht="26">
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="12" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="9" spans="4:6" ht="25.5">
-      <c r="D9" s="42">
-        <v>2</v>
-      </c>
-      <c r="E9" s="42" t="s">
-        <v>87</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="10" spans="4:6">
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="12" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="11" spans="4:6">
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="12" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="12" spans="4:6">
-      <c r="D12" s="42">
-        <v>3</v>
-      </c>
-      <c r="E12" s="42" t="s">
-        <v>136</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="13" spans="4:6">
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="12" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="14" spans="4:6">
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="12" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="15" spans="4:6" ht="25">
-      <c r="D15" s="42">
-        <v>4</v>
-      </c>
-      <c r="E15" s="42" t="s">
-        <v>137</v>
-      </c>
-      <c r="F15" s="13" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="16" spans="4:6" ht="26">
-      <c r="D16" s="43"/>
-      <c r="E16" s="43"/>
-      <c r="F16" s="12" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="17" spans="4:6">
-      <c r="D17" s="43"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="12" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="18" spans="4:6" ht="38">
-      <c r="D18" s="42">
-        <v>5</v>
-      </c>
-      <c r="E18" s="42" t="s">
-        <v>138</v>
-      </c>
-      <c r="F18" s="13" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="19" spans="4:6">
-      <c r="D19" s="43"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="12" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="20" spans="4:6">
-      <c r="D20" s="43"/>
-      <c r="E20" s="43"/>
-      <c r="F20" s="12" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="21" spans="4:6">
-      <c r="D21" s="42">
-        <v>6</v>
-      </c>
-      <c r="E21" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="F21" s="13" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="22" spans="4:6">
-      <c r="D22" s="43"/>
-      <c r="E22" s="43"/>
-      <c r="F22" s="12" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="23" spans="4:6">
-      <c r="D23" s="43"/>
-      <c r="E23" s="43"/>
-      <c r="F23" s="12" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="24" spans="4:6" ht="38">
-      <c r="D24" s="42">
-        <v>7</v>
-      </c>
-      <c r="E24" s="42" t="s">
-        <v>137</v>
-      </c>
-      <c r="F24" s="13" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="25" spans="4:6">
-      <c r="D25" s="43"/>
-      <c r="E25" s="43"/>
-      <c r="F25" s="12" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="26" spans="4:6">
-      <c r="D26" s="43"/>
-      <c r="E26" s="43"/>
-      <c r="F26" s="12" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="27" spans="4:6" ht="26">
-      <c r="D27" s="42">
-        <v>8</v>
-      </c>
-      <c r="E27" s="42" t="s">
-        <v>139</v>
-      </c>
-      <c r="F27" s="13" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="28" spans="4:6" ht="26">
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="12" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="29" spans="4:6">
-      <c r="D29" s="43"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="30" spans="4:6" ht="25">
-      <c r="D30" s="42">
-        <v>9</v>
-      </c>
-      <c r="E30" s="42" t="s">
-        <v>87</v>
-      </c>
-      <c r="F30" s="13" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="31" spans="4:6">
-      <c r="D31" s="43"/>
-      <c r="E31" s="43"/>
-      <c r="F31" s="12" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="32" spans="4:6">
-      <c r="D32" s="43"/>
-      <c r="E32" s="43"/>
-      <c r="F32" s="12" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="33" spans="4:6">
-      <c r="D33" s="42">
-        <v>10</v>
-      </c>
-      <c r="E33" s="42" t="s">
-        <v>87</v>
-      </c>
-      <c r="F33" s="13" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="34" spans="4:6">
-      <c r="D34" s="43"/>
-      <c r="E34" s="43"/>
-      <c r="F34" s="12" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="35" spans="4:6">
-      <c r="D35" s="43"/>
-      <c r="E35" s="43"/>
-      <c r="F35" s="12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="36" spans="4:6" ht="25">
-      <c r="D36" s="42">
-        <v>11</v>
-      </c>
-      <c r="E36" s="42" t="s">
-        <v>140</v>
-      </c>
-      <c r="F36" s="13" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="37" spans="4:6">
-      <c r="D37" s="43"/>
-      <c r="E37" s="43"/>
-      <c r="F37" s="12" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="38" spans="4:6">
-      <c r="D38" s="43"/>
-      <c r="E38" s="43"/>
-      <c r="F38" s="12" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="39" spans="4:6" ht="37.5">
-      <c r="D39" s="42">
-        <v>12</v>
-      </c>
-      <c r="E39" s="42" t="s">
-        <v>141</v>
-      </c>
-      <c r="F39" s="13" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="40" spans="4:6">
-      <c r="D40" s="43"/>
-      <c r="E40" s="43"/>
-      <c r="F40" s="12" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="41" spans="4:6">
-      <c r="D41" s="43"/>
-      <c r="E41" s="43"/>
-      <c r="F41" s="12" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="42" spans="4:6" ht="25">
-      <c r="D42" s="42">
-        <v>13</v>
-      </c>
-      <c r="E42" s="42" t="s">
-        <v>137</v>
-      </c>
-      <c r="F42" s="13" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="43" spans="4:6">
-      <c r="D43" s="43"/>
-      <c r="E43" s="43"/>
-      <c r="F43" s="12" t="s">
+      <c r="F69" s="16" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="70" spans="4:6" ht="26">
+      <c r="D70" s="44"/>
+      <c r="E70" s="44"/>
+      <c r="F70" s="12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="71" spans="4:6">
+      <c r="D71" s="44"/>
+      <c r="E71" s="44"/>
+      <c r="F71" s="12" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="72" spans="4:6">
+      <c r="D72" s="43">
+        <v>23</v>
+      </c>
+      <c r="E72" s="43" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="44" spans="4:6">
-      <c r="D44" s="43"/>
-      <c r="E44" s="43"/>
-      <c r="F44" s="12" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="45" spans="4:6" ht="75.5">
-      <c r="D45" s="42">
-        <v>14</v>
-      </c>
-      <c r="E45" s="42" t="s">
-        <v>142</v>
-      </c>
-      <c r="F45" s="13" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="46" spans="4:6" ht="26">
-      <c r="D46" s="43"/>
-      <c r="E46" s="43"/>
-      <c r="F46" s="12" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="47" spans="4:6">
-      <c r="D47" s="43"/>
-      <c r="E47" s="43"/>
-      <c r="F47" s="12" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="48" spans="4:6" ht="37.5">
-      <c r="D48" s="42">
-        <v>15</v>
-      </c>
-      <c r="E48" s="42" t="s">
-        <v>143</v>
-      </c>
-      <c r="F48" s="13" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="49" spans="4:6" ht="26">
-      <c r="D49" s="43"/>
-      <c r="E49" s="43"/>
-      <c r="F49" s="12" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="50" spans="4:6">
-      <c r="D50" s="43"/>
-      <c r="E50" s="43"/>
-      <c r="F50" s="12" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="51" spans="4:6" ht="25">
-      <c r="D51" s="42">
-        <v>16</v>
-      </c>
-      <c r="E51" s="42" t="s">
-        <v>144</v>
-      </c>
-      <c r="F51" s="13" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="52" spans="4:6">
-      <c r="D52" s="43"/>
-      <c r="E52" s="43"/>
-      <c r="F52" s="12" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="53" spans="4:6">
-      <c r="D53" s="43"/>
-      <c r="E53" s="43"/>
-      <c r="F53" s="12" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="54" spans="4:6" ht="25">
-      <c r="D54" s="42">
-        <v>17</v>
-      </c>
-      <c r="E54" s="42" t="s">
-        <v>144</v>
-      </c>
-      <c r="F54" s="13" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="55" spans="4:6">
-      <c r="D55" s="43"/>
-      <c r="E55" s="43"/>
-      <c r="F55" s="12" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="56" spans="4:6">
-      <c r="D56" s="43"/>
-      <c r="E56" s="43"/>
-      <c r="F56" s="12" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="57" spans="4:6">
-      <c r="D57" s="42">
-        <v>18</v>
-      </c>
-      <c r="E57" s="42" t="s">
-        <v>87</v>
-      </c>
-      <c r="F57" s="13" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="58" spans="4:6">
-      <c r="D58" s="43"/>
-      <c r="E58" s="43"/>
-      <c r="F58" s="12" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="59" spans="4:6">
-      <c r="D59" s="43"/>
-      <c r="E59" s="43"/>
-      <c r="F59" s="12" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="60" spans="4:6" ht="34">
-      <c r="D60" s="42">
-        <v>19</v>
-      </c>
-      <c r="E60" s="42" t="s">
-        <v>87</v>
-      </c>
-      <c r="F60" s="16" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="61" spans="4:6">
-      <c r="D61" s="43"/>
-      <c r="E61" s="43"/>
-      <c r="F61" s="12" t="s">
+      <c r="F72" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="73" spans="4:6" ht="26">
+      <c r="D73" s="44"/>
+      <c r="E73" s="44"/>
+      <c r="F73" s="12" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="62" spans="4:6">
-      <c r="D62" s="43"/>
-      <c r="E62" s="43"/>
-      <c r="F62" s="12" t="s">
+    <row r="74" spans="4:6">
+      <c r="D74" s="44"/>
+      <c r="E74" s="44"/>
+      <c r="F74" s="12" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="63" spans="4:6" ht="34">
-      <c r="D63" s="42">
-        <v>20</v>
-      </c>
-      <c r="E63" s="42" t="s">
-        <v>89</v>
-      </c>
-      <c r="F63" s="16" t="s">
+    <row r="75" spans="4:6">
+      <c r="D75" s="43">
+        <v>24</v>
+      </c>
+      <c r="E75" s="43" t="s">
+        <v>81</v>
+      </c>
+      <c r="F75" s="15" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="76" spans="4:6">
+      <c r="D76" s="44"/>
+      <c r="E76" s="44"/>
+      <c r="F76" s="12" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="64" spans="4:6">
-      <c r="D64" s="43"/>
-      <c r="E64" s="43"/>
-      <c r="F64" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="65" spans="4:6">
-      <c r="D65" s="43"/>
-      <c r="E65" s="43"/>
-      <c r="F65" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="66" spans="4:6" ht="34">
-      <c r="D66" s="42">
-        <v>21</v>
-      </c>
-      <c r="E66" s="42" t="s">
-        <v>89</v>
-      </c>
-      <c r="F66" s="16" t="s">
+    <row r="77" spans="4:6">
+      <c r="D77" s="44"/>
+      <c r="E77" s="44"/>
+      <c r="F77" s="12" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="78" spans="4:6" ht="34">
+      <c r="D78" s="43">
+        <v>25</v>
+      </c>
+      <c r="E78" s="43" t="s">
+        <v>81</v>
+      </c>
+      <c r="F78" s="16" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="79" spans="4:6">
+      <c r="D79" s="44"/>
+      <c r="E79" s="44"/>
+      <c r="F79" s="12" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="67" spans="4:6" ht="26">
-      <c r="D67" s="43"/>
-      <c r="E67" s="43"/>
-      <c r="F67" s="12" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="68" spans="4:6">
-      <c r="D68" s="43"/>
-      <c r="E68" s="43"/>
-      <c r="F68" s="12" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="69" spans="4:6" ht="34">
-      <c r="D69" s="42">
-        <v>22</v>
-      </c>
-      <c r="E69" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="F69" s="16" t="s">
+    <row r="80" spans="4:6">
+      <c r="D80" s="44"/>
+      <c r="E80" s="44"/>
+      <c r="F80" s="12" t="s">
         <v>179</v>
-      </c>
-    </row>
-    <row r="70" spans="4:6" ht="26">
-      <c r="D70" s="43"/>
-      <c r="E70" s="43"/>
-      <c r="F70" s="12" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="71" spans="4:6">
-      <c r="D71" s="43"/>
-      <c r="E71" s="43"/>
-      <c r="F71" s="12" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="72" spans="4:6">
-      <c r="D72" s="42">
-        <v>23</v>
-      </c>
-      <c r="E72" s="42" t="s">
-        <v>120</v>
-      </c>
-      <c r="F72" s="5" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="73" spans="4:6" ht="26">
-      <c r="D73" s="43"/>
-      <c r="E73" s="43"/>
-      <c r="F73" s="12" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="74" spans="4:6">
-      <c r="D74" s="43"/>
-      <c r="E74" s="43"/>
-      <c r="F74" s="12" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="75" spans="4:6">
-      <c r="D75" s="42">
-        <v>24</v>
-      </c>
-      <c r="E75" s="42" t="s">
-        <v>87</v>
-      </c>
-      <c r="F75" s="15" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="76" spans="4:6">
-      <c r="D76" s="43"/>
-      <c r="E76" s="43"/>
-      <c r="F76" s="12" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="77" spans="4:6">
-      <c r="D77" s="43"/>
-      <c r="E77" s="43"/>
-      <c r="F77" s="12" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="78" spans="4:6" ht="34">
-      <c r="D78" s="42">
-        <v>25</v>
-      </c>
-      <c r="E78" s="42" t="s">
-        <v>87</v>
-      </c>
-      <c r="F78" s="16" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="79" spans="4:6">
-      <c r="D79" s="43"/>
-      <c r="E79" s="43"/>
-      <c r="F79" s="12" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="80" spans="4:6">
-      <c r="D80" s="43"/>
-      <c r="E80" s="43"/>
-      <c r="F80" s="12" t="s">
-        <v>185</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="D60:D62"/>
-    <mergeCell ref="E60:E62"/>
-    <mergeCell ref="D72:D74"/>
-    <mergeCell ref="E72:E74"/>
-    <mergeCell ref="D63:D65"/>
-    <mergeCell ref="E63:E65"/>
-    <mergeCell ref="D66:D68"/>
-    <mergeCell ref="E66:E68"/>
-    <mergeCell ref="D69:D71"/>
-    <mergeCell ref="E69:E71"/>
-    <mergeCell ref="D51:D53"/>
-    <mergeCell ref="E51:E53"/>
-    <mergeCell ref="D54:D56"/>
-    <mergeCell ref="E54:E56"/>
-    <mergeCell ref="D57:D59"/>
-    <mergeCell ref="E57:E59"/>
-    <mergeCell ref="D42:D44"/>
-    <mergeCell ref="E42:E44"/>
-    <mergeCell ref="D45:D47"/>
-    <mergeCell ref="E45:E47"/>
-    <mergeCell ref="D48:D50"/>
-    <mergeCell ref="E48:E50"/>
-    <mergeCell ref="D33:D35"/>
-    <mergeCell ref="E33:E35"/>
-    <mergeCell ref="D36:D38"/>
-    <mergeCell ref="E36:E38"/>
-    <mergeCell ref="D39:D41"/>
-    <mergeCell ref="E39:E41"/>
-    <mergeCell ref="D24:D26"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="D27:D29"/>
-    <mergeCell ref="E27:E29"/>
-    <mergeCell ref="D30:D32"/>
-    <mergeCell ref="E30:E32"/>
     <mergeCell ref="D75:D77"/>
     <mergeCell ref="E75:E77"/>
     <mergeCell ref="D78:D80"/>
@@ -43592,6 +43575,40 @@
     <mergeCell ref="E18:E20"/>
     <mergeCell ref="D21:D23"/>
     <mergeCell ref="E21:E23"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="D27:D29"/>
+    <mergeCell ref="E27:E29"/>
+    <mergeCell ref="D30:D32"/>
+    <mergeCell ref="E30:E32"/>
+    <mergeCell ref="D33:D35"/>
+    <mergeCell ref="E33:E35"/>
+    <mergeCell ref="D36:D38"/>
+    <mergeCell ref="E36:E38"/>
+    <mergeCell ref="D39:D41"/>
+    <mergeCell ref="E39:E41"/>
+    <mergeCell ref="D42:D44"/>
+    <mergeCell ref="E42:E44"/>
+    <mergeCell ref="D45:D47"/>
+    <mergeCell ref="E45:E47"/>
+    <mergeCell ref="D48:D50"/>
+    <mergeCell ref="E48:E50"/>
+    <mergeCell ref="D51:D53"/>
+    <mergeCell ref="E51:E53"/>
+    <mergeCell ref="D54:D56"/>
+    <mergeCell ref="E54:E56"/>
+    <mergeCell ref="D57:D59"/>
+    <mergeCell ref="E57:E59"/>
+    <mergeCell ref="D60:D62"/>
+    <mergeCell ref="E60:E62"/>
+    <mergeCell ref="D72:D74"/>
+    <mergeCell ref="E72:E74"/>
+    <mergeCell ref="D63:D65"/>
+    <mergeCell ref="E63:E65"/>
+    <mergeCell ref="D66:D68"/>
+    <mergeCell ref="E66:E68"/>
+    <mergeCell ref="D69:D71"/>
+    <mergeCell ref="E69:E71"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -43614,12 +43631,12 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="B2" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -43672,12 +43689,12 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="B16" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -43685,7 +43702,7 @@
         <v>3</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -43693,7 +43710,7 @@
         <v>4</v>
       </c>
       <c r="B38" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -43701,12 +43718,12 @@
         <v>5</v>
       </c>
       <c r="B47" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="B48" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -43714,12 +43731,12 @@
         <v>6</v>
       </c>
       <c r="B59" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="B60" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -43727,7 +43744,7 @@
         <v>7</v>
       </c>
       <c r="B70" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -43735,17 +43752,17 @@
         <v>8</v>
       </c>
       <c r="B80" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="B81" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="B82" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -43753,12 +43770,12 @@
         <v>9</v>
       </c>
       <c r="B92" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="B93" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -43766,22 +43783,22 @@
         <v>10</v>
       </c>
       <c r="B103" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="B104" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="B105" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="B106" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -43789,7 +43806,7 @@
         <v>11</v>
       </c>
       <c r="B117" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -43797,7 +43814,7 @@
         <v>12</v>
       </c>
       <c r="B133" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -43805,7 +43822,7 @@
         <v>13</v>
       </c>
       <c r="B145" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="156" spans="1:2">
@@ -43813,12 +43830,12 @@
         <v>14</v>
       </c>
       <c r="B156" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="157" spans="1:2">
       <c r="B157" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="169" spans="1:2">
@@ -43826,12 +43843,12 @@
         <v>15</v>
       </c>
       <c r="B169" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="170" spans="1:2">
       <c r="B170" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="181" spans="1:2">
@@ -43839,12 +43856,12 @@
         <v>16</v>
       </c>
       <c r="B181" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="182" spans="1:2">
       <c r="B182" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
     </row>
     <row r="192" spans="1:2">
@@ -43852,12 +43869,12 @@
         <v>17</v>
       </c>
       <c r="B192" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="193" spans="1:2">
       <c r="B193" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="203" spans="1:2">
@@ -43865,12 +43882,12 @@
         <v>18</v>
       </c>
       <c r="B203" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="204" spans="1:2">
       <c r="B204" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
     </row>
     <row r="214" spans="1:2">
@@ -43878,17 +43895,17 @@
         <v>19</v>
       </c>
       <c r="B214" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
     </row>
     <row r="215" spans="1:2">
       <c r="B215" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="216" spans="1:2">
       <c r="B216" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="230" spans="1:2">
@@ -43896,7 +43913,7 @@
         <v>20</v>
       </c>
       <c r="B230" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="243" spans="1:2">
@@ -43904,7 +43921,7 @@
         <v>21</v>
       </c>
       <c r="B243" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
     </row>
     <row r="254" spans="1:2">
@@ -43912,12 +43929,12 @@
         <v>22</v>
       </c>
       <c r="B254" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="255" spans="1:2">
       <c r="B255" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="266" spans="1:2">
@@ -43925,12 +43942,12 @@
         <v>23</v>
       </c>
       <c r="B266" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
     </row>
     <row r="267" spans="1:2">
       <c r="B267" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="280" spans="1:2">
@@ -43938,17 +43955,17 @@
         <v>24</v>
       </c>
       <c r="B280" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="281" spans="1:2">
       <c r="B281" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="282" spans="1:2">
       <c r="B282" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
     </row>
     <row r="293" spans="1:2">
@@ -43956,12 +43973,12 @@
         <v>25</v>
       </c>
       <c r="B293" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="294" spans="1:2">
       <c r="B294" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
need header 주석 추가
</commit_message>
<xml_diff>
--- a/exerdProject/기능명세서.xlsx
+++ b/exerdProject/기능명세서.xlsx
@@ -11071,12 +11071,6 @@
     <t>/srch/list/mem/do.admin</t>
   </si>
   <si>
-    <t>/fix/mem/do.go</t>
-  </si>
-  <si>
-    <t>/del/mem/do.go</t>
-  </si>
-  <si>
     <t>/acvt/mem/do</t>
   </si>
   <si>
@@ -11285,6 +11279,14 @@
   </si>
   <si>
     <t>/fix/sche/do.go</t>
+  </si>
+  <si>
+    <t>/fix/mem/do.my</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/del/mem/do.my</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -11663,6 +11665,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -11708,7 +11711,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -11774,7 +11776,7 @@
         <xdr:cNvPr id="3" name="그림 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{72F30C73-F9FC-4F38-BA21-6FBBC4E49CDB}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72F30C73-F9FC-4F38-BA21-6FBBC4E49CDB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11824,7 +11826,7 @@
         <xdr:cNvPr id="5" name="그림 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5BB94D47-326F-4819-8971-AA13705ADEA4}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5BB94D47-326F-4819-8971-AA13705ADEA4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11874,7 +11876,7 @@
         <xdr:cNvPr id="7" name="그림 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{59C13640-91FA-4E80-824E-E4D9C44B5BED}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59C13640-91FA-4E80-824E-E4D9C44B5BED}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11924,7 +11926,7 @@
         <xdr:cNvPr id="9" name="그림 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C4A3605E-7644-45D4-8DE6-84FD004B3F4C}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4A3605E-7644-45D4-8DE6-84FD004B3F4C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11974,7 +11976,7 @@
         <xdr:cNvPr id="11" name="그림 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{62DD966B-C63A-459D-B9C1-C4D087351D8E}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62DD966B-C63A-459D-B9C1-C4D087351D8E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12024,7 +12026,7 @@
         <xdr:cNvPr id="13" name="그림 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A1FEB21B-F265-43E5-BC0F-5A5C3072778D}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1FEB21B-F265-43E5-BC0F-5A5C3072778D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12074,7 +12076,7 @@
         <xdr:cNvPr id="15" name="그림 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{82167F25-CE0C-4328-B74B-67C4A9238083}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82167F25-CE0C-4328-B74B-67C4A9238083}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12124,7 +12126,7 @@
         <xdr:cNvPr id="17" name="그림 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F83AB63C-A07B-4B7E-AB95-B45645F50602}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F83AB63C-A07B-4B7E-AB95-B45645F50602}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12174,7 +12176,7 @@
         <xdr:cNvPr id="19" name="그림 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{433948DD-2AD1-4AC9-B842-63A78A067A70}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{433948DD-2AD1-4AC9-B842-63A78A067A70}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12224,7 +12226,7 @@
         <xdr:cNvPr id="21" name="그림 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{082B1200-C085-4FA7-BE82-27A6BEA6E852}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{082B1200-C085-4FA7-BE82-27A6BEA6E852}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12274,7 +12276,7 @@
         <xdr:cNvPr id="23" name="그림 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E7A074D7-8F92-4F0A-8B56-B91E2CBC3825}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7A074D7-8F92-4F0A-8B56-B91E2CBC3825}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12324,7 +12326,7 @@
         <xdr:cNvPr id="25" name="그림 24">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{53A77203-91F8-463E-8B1B-039C3269D532}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53A77203-91F8-463E-8B1B-039C3269D532}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12374,7 +12376,7 @@
         <xdr:cNvPr id="27" name="그림 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C7118837-89E4-446F-97EF-B5D9FB7F2FB4}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7118837-89E4-446F-97EF-B5D9FB7F2FB4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12424,7 +12426,7 @@
         <xdr:cNvPr id="29" name="그림 28">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8737BCA7-F78B-4B91-A595-9653D635C7D5}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8737BCA7-F78B-4B91-A595-9653D635C7D5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12474,7 +12476,7 @@
         <xdr:cNvPr id="31" name="그림 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B2AF5EE9-C4ED-4408-A5F6-28A0E9417D7E}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2AF5EE9-C4ED-4408-A5F6-28A0E9417D7E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12524,7 +12526,7 @@
         <xdr:cNvPr id="33" name="그림 32">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6B138BD1-1A05-4487-B0A5-BADA3B2BF1C1}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B138BD1-1A05-4487-B0A5-BADA3B2BF1C1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12574,7 +12576,7 @@
         <xdr:cNvPr id="35" name="그림 34">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B8EEEE74-6CDD-4AD0-AA9E-B9957525B74B}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8EEEE74-6CDD-4AD0-AA9E-B9957525B74B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12624,7 +12626,7 @@
         <xdr:cNvPr id="37" name="그림 36">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E3433636-4576-43A7-8AD9-BB8E1A1E1AD8}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3433636-4576-43A7-8AD9-BB8E1A1E1AD8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12674,7 +12676,7 @@
         <xdr:cNvPr id="39" name="그림 38">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3C4A0C2B-4389-4D57-A3E0-2D04338083F9}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C4A0C2B-4389-4D57-A3E0-2D04338083F9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12724,7 +12726,7 @@
         <xdr:cNvPr id="41" name="그림 40">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{89BC0C82-65FA-44E5-A832-010C0FF640FC}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89BC0C82-65FA-44E5-A832-010C0FF640FC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12774,7 +12776,7 @@
         <xdr:cNvPr id="43" name="그림 42">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{31F9904A-3271-4FA6-8901-1D90AB0455FB}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31F9904A-3271-4FA6-8901-1D90AB0455FB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12824,7 +12826,7 @@
         <xdr:cNvPr id="45" name="그림 44">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0683093B-4E9B-475F-811C-7650A098856C}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0683093B-4E9B-475F-811C-7650A098856C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12874,7 +12876,7 @@
         <xdr:cNvPr id="47" name="그림 46">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2009715D-AB1E-470A-AA53-9931BA579CDC}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2009715D-AB1E-470A-AA53-9931BA579CDC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12924,7 +12926,7 @@
         <xdr:cNvPr id="49" name="그림 48">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{18FFBF34-399E-4097-A49B-AAEB71760605}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18FFBF34-399E-4097-A49B-AAEB71760605}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12974,7 +12976,7 @@
         <xdr:cNvPr id="51" name="그림 50">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D6310A5F-8868-44D1-AD9B-A1998B7650F4}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6310A5F-8868-44D1-AD9B-A1998B7650F4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13264,7 +13266,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -13274,8 +13276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD1016"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="K61" sqref="K61"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="17"/>
@@ -13297,23 +13299,23 @@
     </row>
     <row r="2" spans="1:30">
       <c r="B2" s="19" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C2" s="4"/>
     </row>
     <row r="3" spans="1:30">
       <c r="B3" s="19" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="4" spans="1:30">
       <c r="B4" s="42" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="5" spans="1:30">
       <c r="B5" s="19" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="6" spans="1:30" s="37" customFormat="1">
@@ -13351,17 +13353,17 @@
     </row>
     <row r="7" spans="1:30" ht="17.399999999999999" customHeight="1">
       <c r="A7" s="3"/>
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="47"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="47"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="47"/>
-      <c r="H7" s="47"/>
-      <c r="I7" s="47"/>
-      <c r="J7" s="47"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="48"/>
+      <c r="H7" s="48"/>
+      <c r="I7" s="48"/>
+      <c r="J7" s="48"/>
       <c r="K7" s="40"/>
       <c r="L7" s="40"/>
       <c r="M7" s="40"/>
@@ -13385,15 +13387,15 @@
     </row>
     <row r="8" spans="1:30" ht="17.399999999999999" customHeight="1">
       <c r="A8" s="3"/>
-      <c r="B8" s="47"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="47"/>
-      <c r="I8" s="47"/>
-      <c r="J8" s="47"/>
+      <c r="B8" s="48"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="48"/>
+      <c r="H8" s="48"/>
+      <c r="I8" s="48"/>
+      <c r="J8" s="48"/>
       <c r="K8" s="40" t="s">
         <v>293</v>
       </c>
@@ -13433,15 +13435,15 @@
     </row>
     <row r="9" spans="1:30" ht="18" customHeight="1">
       <c r="A9" s="3"/>
-      <c r="B9" s="47"/>
-      <c r="C9" s="47"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="47"/>
-      <c r="H9" s="47"/>
-      <c r="I9" s="47"/>
-      <c r="J9" s="47"/>
+      <c r="B9" s="48"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="48"/>
+      <c r="J9" s="48"/>
       <c r="K9" s="40"/>
       <c r="L9" s="40"/>
       <c r="M9" s="40"/>
@@ -13467,10 +13469,10 @@
     </row>
     <row r="10" spans="1:30" ht="18" customHeight="1">
       <c r="A10" s="3"/>
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="46"/>
+      <c r="C10" s="47"/>
       <c r="D10" s="1" t="s">
         <v>17</v>
       </c>
@@ -13515,8 +13517,8 @@
     </row>
     <row r="11" spans="1:30">
       <c r="A11" s="3"/>
-      <c r="B11" s="46"/>
-      <c r="C11" s="46"/>
+      <c r="B11" s="47"/>
+      <c r="C11" s="47"/>
       <c r="D11" s="1" t="s">
         <v>21</v>
       </c>
@@ -13561,8 +13563,8 @@
     </row>
     <row r="12" spans="1:30">
       <c r="A12" s="3"/>
-      <c r="B12" s="46"/>
-      <c r="C12" s="46"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="47"/>
       <c r="D12" s="1" t="s">
         <v>22</v>
       </c>
@@ -13607,8 +13609,8 @@
     </row>
     <row r="13" spans="1:30">
       <c r="A13" s="3"/>
-      <c r="B13" s="46"/>
-      <c r="C13" s="46"/>
+      <c r="B13" s="47"/>
+      <c r="C13" s="47"/>
       <c r="D13" s="1" t="s">
         <v>23</v>
       </c>
@@ -13625,7 +13627,7 @@
         <v>20</v>
       </c>
       <c r="K13" s="34" t="s">
-        <v>301</v>
+        <v>361</v>
       </c>
       <c r="L13" s="34"/>
       <c r="M13" s="34"/>
@@ -13653,8 +13655,8 @@
     </row>
     <row r="14" spans="1:30">
       <c r="A14" s="3"/>
-      <c r="B14" s="46"/>
-      <c r="C14" s="46"/>
+      <c r="B14" s="47"/>
+      <c r="C14" s="47"/>
       <c r="D14" s="1" t="s">
         <v>24</v>
       </c>
@@ -13671,7 +13673,7 @@
         <v>20</v>
       </c>
       <c r="K14" s="34" t="s">
-        <v>302</v>
+        <v>362</v>
       </c>
       <c r="L14" s="34"/>
       <c r="M14" s="34"/>
@@ -13699,8 +13701,8 @@
     </row>
     <row r="15" spans="1:30">
       <c r="A15" s="3"/>
-      <c r="B15" s="46"/>
-      <c r="C15" s="46"/>
+      <c r="B15" s="47"/>
+      <c r="C15" s="47"/>
       <c r="D15" s="1" t="s">
         <v>25</v>
       </c>
@@ -13717,7 +13719,7 @@
         <v>20</v>
       </c>
       <c r="K15" s="34" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="L15" s="34"/>
       <c r="M15" s="34"/>
@@ -13745,8 +13747,8 @@
     </row>
     <row r="16" spans="1:30">
       <c r="A16" s="3"/>
-      <c r="B16" s="46"/>
-      <c r="C16" s="46"/>
+      <c r="B16" s="47"/>
+      <c r="C16" s="47"/>
       <c r="D16" s="1" t="s">
         <v>26</v>
       </c>
@@ -13791,8 +13793,8 @@
     </row>
     <row r="17" spans="1:30">
       <c r="A17" s="3"/>
-      <c r="B17" s="46"/>
-      <c r="C17" s="46"/>
+      <c r="B17" s="47"/>
+      <c r="C17" s="47"/>
       <c r="D17" s="1" t="s">
         <v>27</v>
       </c>
@@ -13833,10 +13835,10 @@
     </row>
     <row r="18" spans="1:30" ht="17.399999999999999" customHeight="1">
       <c r="A18" s="3"/>
-      <c r="B18" s="49" t="s">
+      <c r="B18" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="50"/>
+      <c r="C18" s="51"/>
       <c r="D18" s="2" t="s">
         <v>29</v>
       </c>
@@ -13853,7 +13855,7 @@
         <v>20</v>
       </c>
       <c r="K18" s="34" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="L18" s="34"/>
       <c r="M18" s="34"/>
@@ -13881,8 +13883,8 @@
     </row>
     <row r="19" spans="1:30">
       <c r="A19" s="3"/>
-      <c r="B19" s="51"/>
-      <c r="C19" s="52"/>
+      <c r="B19" s="52"/>
+      <c r="C19" s="53"/>
       <c r="D19" s="2" t="s">
         <v>30</v>
       </c>
@@ -13899,7 +13901,7 @@
         <v>20</v>
       </c>
       <c r="K19" s="34" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="L19" s="34"/>
       <c r="M19" s="34"/>
@@ -13927,8 +13929,8 @@
     </row>
     <row r="20" spans="1:30">
       <c r="A20" s="3"/>
-      <c r="B20" s="51"/>
-      <c r="C20" s="52"/>
+      <c r="B20" s="52"/>
+      <c r="C20" s="53"/>
       <c r="D20" s="2" t="s">
         <v>31</v>
       </c>
@@ -13945,7 +13947,7 @@
         <v>20</v>
       </c>
       <c r="K20" s="34" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="L20" s="34"/>
       <c r="M20" s="34"/>
@@ -13953,7 +13955,7 @@
         <v>249</v>
       </c>
       <c r="O20" s="5" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="P20" s="19"/>
       <c r="Q20" s="19"/>
@@ -13973,8 +13975,8 @@
     </row>
     <row r="21" spans="1:30">
       <c r="A21" s="3"/>
-      <c r="B21" s="51"/>
-      <c r="C21" s="52"/>
+      <c r="B21" s="52"/>
+      <c r="C21" s="53"/>
       <c r="D21" s="2" t="s">
         <v>32</v>
       </c>
@@ -13991,7 +13993,7 @@
         <v>20</v>
       </c>
       <c r="K21" s="34" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="L21" s="34"/>
       <c r="M21" s="34"/>
@@ -14019,8 +14021,8 @@
     </row>
     <row r="22" spans="1:30">
       <c r="A22" s="3"/>
-      <c r="B22" s="51"/>
-      <c r="C22" s="52"/>
+      <c r="B22" s="52"/>
+      <c r="C22" s="53"/>
       <c r="D22" s="2" t="s">
         <v>33</v>
       </c>
@@ -14037,7 +14039,7 @@
         <v>20</v>
       </c>
       <c r="K22" s="34" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="L22" s="34"/>
       <c r="M22" s="34"/>
@@ -14065,8 +14067,8 @@
     </row>
     <row r="23" spans="1:30">
       <c r="A23" s="3"/>
-      <c r="B23" s="51"/>
-      <c r="C23" s="52"/>
+      <c r="B23" s="52"/>
+      <c r="C23" s="53"/>
       <c r="D23" s="2" t="s">
         <v>34</v>
       </c>
@@ -14083,7 +14085,7 @@
         <v>20</v>
       </c>
       <c r="K23" s="34" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="L23" s="34"/>
       <c r="M23" s="34"/>
@@ -14111,8 +14113,8 @@
     </row>
     <row r="24" spans="1:30">
       <c r="A24" s="3"/>
-      <c r="B24" s="51"/>
-      <c r="C24" s="52"/>
+      <c r="B24" s="52"/>
+      <c r="C24" s="53"/>
       <c r="D24" s="2" t="s">
         <v>35</v>
       </c>
@@ -14129,7 +14131,7 @@
         <v>20</v>
       </c>
       <c r="K24" s="34" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="L24" s="34"/>
       <c r="M24" s="34"/>
@@ -14137,7 +14139,7 @@
         <v>280</v>
       </c>
       <c r="O24" s="5" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="P24" s="19"/>
       <c r="Q24" s="19"/>
@@ -14157,10 +14159,10 @@
     </row>
     <row r="25" spans="1:30" ht="18" customHeight="1">
       <c r="A25" s="19" t="s">
-        <v>314</v>
-      </c>
-      <c r="B25" s="51"/>
-      <c r="C25" s="52"/>
+        <v>312</v>
+      </c>
+      <c r="B25" s="52"/>
+      <c r="C25" s="53"/>
       <c r="D25" s="2" t="s">
         <v>36</v>
       </c>
@@ -14177,7 +14179,7 @@
         <v>20</v>
       </c>
       <c r="K25" s="34" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="L25" s="34"/>
       <c r="M25" s="34"/>
@@ -14205,10 +14207,10 @@
     </row>
     <row r="26" spans="1:30">
       <c r="A26" s="19" t="s">
-        <v>314</v>
-      </c>
-      <c r="B26" s="51"/>
-      <c r="C26" s="52"/>
+        <v>312</v>
+      </c>
+      <c r="B26" s="52"/>
+      <c r="C26" s="53"/>
       <c r="D26" s="2" t="s">
         <v>37</v>
       </c>
@@ -14225,7 +14227,7 @@
         <v>20</v>
       </c>
       <c r="K26" s="34" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="L26" s="34"/>
       <c r="M26" s="34"/>
@@ -14253,8 +14255,8 @@
     </row>
     <row r="27" spans="1:30">
       <c r="A27" s="3"/>
-      <c r="B27" s="51"/>
-      <c r="C27" s="52"/>
+      <c r="B27" s="52"/>
+      <c r="C27" s="53"/>
       <c r="D27" s="2" t="s">
         <v>38</v>
       </c>
@@ -14271,7 +14273,7 @@
         <v>20</v>
       </c>
       <c r="K27" s="34" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="L27" s="34"/>
       <c r="M27" s="34"/>
@@ -14299,8 +14301,8 @@
     </row>
     <row r="28" spans="1:30">
       <c r="A28" s="3"/>
-      <c r="B28" s="51"/>
-      <c r="C28" s="52"/>
+      <c r="B28" s="52"/>
+      <c r="C28" s="53"/>
       <c r="D28" s="2" t="s">
         <v>39</v>
       </c>
@@ -14317,7 +14319,7 @@
         <v>20</v>
       </c>
       <c r="K28" s="34" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="L28" s="34"/>
       <c r="M28" s="34"/>
@@ -14335,10 +14337,10 @@
       <c r="U28" s="3"/>
       <c r="V28" s="3"/>
       <c r="W28" s="3"/>
-      <c r="X28" s="45" t="s">
+      <c r="X28" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="Y28" s="45"/>
+      <c r="Y28" s="46"/>
       <c r="Z28" s="3"/>
       <c r="AA28" s="3"/>
       <c r="AB28" s="3"/>
@@ -14347,10 +14349,10 @@
     </row>
     <row r="29" spans="1:30">
       <c r="A29" s="3"/>
-      <c r="B29" s="53"/>
-      <c r="C29" s="54"/>
+      <c r="B29" s="54"/>
+      <c r="C29" s="55"/>
       <c r="D29" s="2" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="E29" s="28"/>
       <c r="F29" s="28"/>
@@ -14365,15 +14367,15 @@
         <v>20</v>
       </c>
       <c r="K29" s="34" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="L29" s="34"/>
       <c r="M29" s="34"/>
       <c r="N29" s="34" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="O29" s="5" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="P29" s="19"/>
       <c r="Q29" s="19"/>
@@ -14393,10 +14395,10 @@
     </row>
     <row r="30" spans="1:30" ht="18" customHeight="1">
       <c r="A30" s="3"/>
-      <c r="B30" s="46" t="s">
+      <c r="B30" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="C30" s="46"/>
+      <c r="C30" s="47"/>
       <c r="D30" s="1" t="s">
         <v>41</v>
       </c>
@@ -14413,7 +14415,7 @@
         <v>20</v>
       </c>
       <c r="K30" s="34" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="L30" s="34"/>
       <c r="M30" s="34"/>
@@ -14441,8 +14443,8 @@
     </row>
     <row r="31" spans="1:30">
       <c r="A31" s="3"/>
-      <c r="B31" s="46"/>
-      <c r="C31" s="46"/>
+      <c r="B31" s="47"/>
+      <c r="C31" s="47"/>
       <c r="D31" s="1" t="s">
         <v>42</v>
       </c>
@@ -14459,7 +14461,7 @@
         <v>20</v>
       </c>
       <c r="K31" s="34" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="L31" s="34"/>
       <c r="M31" s="34"/>
@@ -14487,8 +14489,8 @@
     </row>
     <row r="32" spans="1:30" ht="18" customHeight="1">
       <c r="A32" s="3"/>
-      <c r="B32" s="46"/>
-      <c r="C32" s="46"/>
+      <c r="B32" s="47"/>
+      <c r="C32" s="47"/>
       <c r="D32" s="1" t="s">
         <v>43</v>
       </c>
@@ -14505,7 +14507,7 @@
         <v>20</v>
       </c>
       <c r="K32" s="34" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="L32" s="34"/>
       <c r="M32" s="34"/>
@@ -14533,8 +14535,8 @@
     </row>
     <row r="33" spans="1:30">
       <c r="A33" s="3"/>
-      <c r="B33" s="46"/>
-      <c r="C33" s="46"/>
+      <c r="B33" s="47"/>
+      <c r="C33" s="47"/>
       <c r="D33" s="1" t="s">
         <v>44</v>
       </c>
@@ -14551,7 +14553,7 @@
         <v>20</v>
       </c>
       <c r="K33" s="34" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="L33" s="34"/>
       <c r="M33" s="34"/>
@@ -14579,10 +14581,10 @@
     </row>
     <row r="34" spans="1:30">
       <c r="A34" s="3" t="s">
-        <v>332</v>
-      </c>
-      <c r="B34" s="46"/>
-      <c r="C34" s="46"/>
+        <v>330</v>
+      </c>
+      <c r="B34" s="47"/>
+      <c r="C34" s="47"/>
       <c r="D34" s="1" t="s">
         <v>45</v>
       </c>
@@ -14599,7 +14601,7 @@
         <v>20</v>
       </c>
       <c r="K34" s="34" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="L34" s="34"/>
       <c r="M34" s="34"/>
@@ -14629,10 +14631,10 @@
     </row>
     <row r="35" spans="1:30" ht="18" customHeight="1">
       <c r="A35" s="3"/>
-      <c r="B35" s="48" t="s">
+      <c r="B35" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="C35" s="48"/>
+      <c r="C35" s="49"/>
       <c r="D35" s="2" t="s">
         <v>48</v>
       </c>
@@ -14649,7 +14651,7 @@
         <v>20</v>
       </c>
       <c r="K35" s="34" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="L35" s="34"/>
       <c r="M35" s="34"/>
@@ -14657,7 +14659,7 @@
         <v>260</v>
       </c>
       <c r="O35" s="36" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="P35" s="19"/>
       <c r="Q35" s="19"/>
@@ -14677,8 +14679,8 @@
     </row>
     <row r="36" spans="1:30">
       <c r="A36" s="3"/>
-      <c r="B36" s="48"/>
-      <c r="C36" s="48"/>
+      <c r="B36" s="49"/>
+      <c r="C36" s="49"/>
       <c r="D36" s="2" t="s">
         <v>226</v>
       </c>
@@ -14695,7 +14697,7 @@
         <v>20</v>
       </c>
       <c r="K36" s="34" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="L36" s="34"/>
       <c r="M36" s="34"/>
@@ -14723,8 +14725,8 @@
     </row>
     <row r="37" spans="1:30">
       <c r="A37" s="3"/>
-      <c r="B37" s="48"/>
-      <c r="C37" s="48"/>
+      <c r="B37" s="49"/>
+      <c r="C37" s="49"/>
       <c r="D37" s="2" t="s">
         <v>229</v>
       </c>
@@ -14741,7 +14743,7 @@
         <v>20</v>
       </c>
       <c r="K37" s="34" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="L37" s="34"/>
       <c r="M37" s="34"/>
@@ -14769,8 +14771,8 @@
     </row>
     <row r="38" spans="1:30">
       <c r="A38" s="3"/>
-      <c r="B38" s="48"/>
-      <c r="C38" s="48"/>
+      <c r="B38" s="49"/>
+      <c r="C38" s="49"/>
       <c r="D38" s="2" t="s">
         <v>49</v>
       </c>
@@ -14809,8 +14811,8 @@
     </row>
     <row r="39" spans="1:30">
       <c r="A39" s="3"/>
-      <c r="B39" s="48"/>
-      <c r="C39" s="48"/>
+      <c r="B39" s="49"/>
+      <c r="C39" s="49"/>
       <c r="D39" s="2" t="s">
         <v>50</v>
       </c>
@@ -14827,7 +14829,7 @@
         <v>20</v>
       </c>
       <c r="K39" s="34" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="L39" s="34"/>
       <c r="M39" s="34"/>
@@ -14835,7 +14837,7 @@
         <v>263</v>
       </c>
       <c r="O39" s="19" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="P39" s="19"/>
       <c r="Q39" s="19"/>
@@ -14855,8 +14857,8 @@
     </row>
     <row r="40" spans="1:30" ht="17.399999999999999" customHeight="1">
       <c r="A40" s="3"/>
-      <c r="B40" s="48"/>
-      <c r="C40" s="48"/>
+      <c r="B40" s="49"/>
+      <c r="C40" s="49"/>
       <c r="D40" s="2" t="s">
         <v>51</v>
       </c>
@@ -14873,7 +14875,7 @@
         <v>20</v>
       </c>
       <c r="K40" s="34" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="L40" s="34"/>
       <c r="M40" s="34"/>
@@ -14901,8 +14903,8 @@
     </row>
     <row r="41" spans="1:30">
       <c r="A41" s="3"/>
-      <c r="B41" s="48"/>
-      <c r="C41" s="48"/>
+      <c r="B41" s="49"/>
+      <c r="C41" s="49"/>
       <c r="D41" s="2" t="s">
         <v>52</v>
       </c>
@@ -14919,7 +14921,7 @@
         <v>20</v>
       </c>
       <c r="K41" s="34" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="L41" s="34"/>
       <c r="M41" s="34"/>
@@ -14927,7 +14929,7 @@
         <v>266</v>
       </c>
       <c r="O41" s="19" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="P41" s="19"/>
       <c r="Q41" s="19"/>
@@ -14947,10 +14949,10 @@
     </row>
     <row r="42" spans="1:30">
       <c r="A42" s="3"/>
-      <c r="B42" s="48"/>
-      <c r="C42" s="48"/>
+      <c r="B42" s="49"/>
+      <c r="C42" s="49"/>
       <c r="D42" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E42" s="28"/>
       <c r="F42" s="28"/>
@@ -14965,15 +14967,15 @@
         <v>20</v>
       </c>
       <c r="K42" s="34" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="L42" s="34"/>
       <c r="M42" s="34"/>
       <c r="N42" s="34" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="O42" s="42" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="P42" s="19"/>
       <c r="Q42" s="19"/>
@@ -14993,8 +14995,8 @@
     </row>
     <row r="43" spans="1:30">
       <c r="A43" s="3"/>
-      <c r="B43" s="48"/>
-      <c r="C43" s="48"/>
+      <c r="B43" s="49"/>
+      <c r="C43" s="49"/>
       <c r="D43" s="2" t="s">
         <v>53</v>
       </c>
@@ -15033,10 +15035,10 @@
     </row>
     <row r="44" spans="1:30" ht="18" customHeight="1">
       <c r="A44" s="3"/>
-      <c r="B44" s="46" t="s">
-        <v>334</v>
-      </c>
-      <c r="C44" s="46"/>
+      <c r="B44" s="47" t="s">
+        <v>332</v>
+      </c>
+      <c r="C44" s="47"/>
       <c r="D44" s="1" t="s">
         <v>54</v>
       </c>
@@ -15052,10 +15054,10 @@
       <c r="J44" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="K44" s="55" t="s">
-        <v>348</v>
-      </c>
-      <c r="L44" s="56"/>
+      <c r="K44" s="56" t="s">
+        <v>346</v>
+      </c>
+      <c r="L44" s="57"/>
       <c r="M44" s="34"/>
       <c r="N44" s="34" t="s">
         <v>237</v>
@@ -15081,8 +15083,8 @@
     </row>
     <row r="45" spans="1:30" ht="18" customHeight="1">
       <c r="A45" s="3"/>
-      <c r="B45" s="46"/>
-      <c r="C45" s="46"/>
+      <c r="B45" s="47"/>
+      <c r="C45" s="47"/>
       <c r="D45" s="1" t="s">
         <v>211</v>
       </c>
@@ -15098,8 +15100,8 @@
       <c r="J45" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="K45" s="55"/>
-      <c r="L45" s="56"/>
+      <c r="K45" s="56"/>
+      <c r="L45" s="57"/>
       <c r="M45" s="34"/>
       <c r="N45" s="34" t="s">
         <v>238</v>
@@ -15125,8 +15127,8 @@
     </row>
     <row r="46" spans="1:30">
       <c r="A46" s="3"/>
-      <c r="B46" s="46"/>
-      <c r="C46" s="46"/>
+      <c r="B46" s="47"/>
+      <c r="C46" s="47"/>
       <c r="D46" s="1" t="s">
         <v>227</v>
       </c>
@@ -15143,7 +15145,7 @@
         <v>20</v>
       </c>
       <c r="K46" s="34" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="L46" s="34"/>
       <c r="M46" s="34"/>
@@ -15171,8 +15173,8 @@
     </row>
     <row r="47" spans="1:30">
       <c r="A47" s="3"/>
-      <c r="B47" s="46"/>
-      <c r="C47" s="46"/>
+      <c r="B47" s="47"/>
+      <c r="C47" s="47"/>
       <c r="D47" s="1" t="s">
         <v>213</v>
       </c>
@@ -15189,7 +15191,7 @@
         <v>20</v>
       </c>
       <c r="K47" s="34" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="L47" s="34"/>
       <c r="M47" s="34"/>
@@ -15217,8 +15219,8 @@
     </row>
     <row r="48" spans="1:30">
       <c r="A48" s="3"/>
-      <c r="B48" s="46"/>
-      <c r="C48" s="46"/>
+      <c r="B48" s="47"/>
+      <c r="C48" s="47"/>
       <c r="D48" s="1" t="s">
         <v>55</v>
       </c>
@@ -15235,7 +15237,7 @@
         <v>20</v>
       </c>
       <c r="K48" s="34" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="L48" s="34"/>
       <c r="M48" s="34"/>
@@ -15263,8 +15265,8 @@
     </row>
     <row r="49" spans="1:30">
       <c r="A49" s="3"/>
-      <c r="B49" s="46"/>
-      <c r="C49" s="46"/>
+      <c r="B49" s="47"/>
+      <c r="C49" s="47"/>
       <c r="D49" s="1" t="s">
         <v>56</v>
       </c>
@@ -15280,10 +15282,10 @@
       <c r="J49" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="K49" s="55" t="s">
-        <v>352</v>
-      </c>
-      <c r="L49" s="56"/>
+      <c r="K49" s="56" t="s">
+        <v>350</v>
+      </c>
+      <c r="L49" s="57"/>
       <c r="M49" s="34"/>
       <c r="N49" s="34" t="s">
         <v>269</v>
@@ -15309,8 +15311,8 @@
     </row>
     <row r="50" spans="1:30">
       <c r="A50" s="3"/>
-      <c r="B50" s="46"/>
-      <c r="C50" s="46"/>
+      <c r="B50" s="47"/>
+      <c r="C50" s="47"/>
       <c r="D50" s="1" t="s">
         <v>216</v>
       </c>
@@ -15326,8 +15328,8 @@
       <c r="J50" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="K50" s="55"/>
-      <c r="L50" s="56"/>
+      <c r="K50" s="56"/>
+      <c r="L50" s="57"/>
       <c r="M50" s="34"/>
       <c r="N50" s="34" t="s">
         <v>240</v>
@@ -15353,8 +15355,8 @@
     </row>
     <row r="51" spans="1:30">
       <c r="A51" s="3"/>
-      <c r="B51" s="46"/>
-      <c r="C51" s="46"/>
+      <c r="B51" s="47"/>
+      <c r="C51" s="47"/>
       <c r="D51" s="1" t="s">
         <v>57</v>
       </c>
@@ -15371,15 +15373,15 @@
         <v>20</v>
       </c>
       <c r="K51" s="34" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="L51" s="34"/>
       <c r="M51" s="34"/>
       <c r="N51" s="34" t="s">
         <v>270</v>
       </c>
-      <c r="O51" s="59" t="s">
-        <v>346</v>
+      <c r="O51" s="44" t="s">
+        <v>344</v>
       </c>
       <c r="P51" s="19"/>
       <c r="Q51" s="19"/>
@@ -15399,8 +15401,8 @@
     </row>
     <row r="52" spans="1:30">
       <c r="A52" s="3"/>
-      <c r="B52" s="46"/>
-      <c r="C52" s="46"/>
+      <c r="B52" s="47"/>
+      <c r="C52" s="47"/>
       <c r="D52" s="1" t="s">
         <v>58</v>
       </c>
@@ -15417,7 +15419,7 @@
         <v>20</v>
       </c>
       <c r="K52" s="34" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="L52" s="34"/>
       <c r="M52" s="34"/>
@@ -15425,7 +15427,7 @@
         <v>271</v>
       </c>
       <c r="O52" s="19" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="P52" s="19"/>
       <c r="Q52" s="19"/>
@@ -15445,10 +15447,10 @@
     </row>
     <row r="53" spans="1:30" ht="18" customHeight="1">
       <c r="A53" s="3"/>
-      <c r="B53" s="48" t="s">
+      <c r="B53" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="C53" s="48"/>
+      <c r="C53" s="49"/>
       <c r="D53" s="2" t="s">
         <v>60</v>
       </c>
@@ -15465,7 +15467,7 @@
         <v>20</v>
       </c>
       <c r="K53" s="34" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="L53" s="34"/>
       <c r="M53" s="34"/>
@@ -15493,8 +15495,8 @@
     </row>
     <row r="54" spans="1:30">
       <c r="A54" s="3"/>
-      <c r="B54" s="48"/>
-      <c r="C54" s="48"/>
+      <c r="B54" s="49"/>
+      <c r="C54" s="49"/>
       <c r="D54" s="2" t="s">
         <v>61</v>
       </c>
@@ -15511,7 +15513,7 @@
         <v>20</v>
       </c>
       <c r="K54" s="34" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="L54" s="34"/>
       <c r="M54" s="34"/>
@@ -15539,8 +15541,8 @@
     </row>
     <row r="55" spans="1:30">
       <c r="A55" s="3"/>
-      <c r="B55" s="48"/>
-      <c r="C55" s="48"/>
+      <c r="B55" s="49"/>
+      <c r="C55" s="49"/>
       <c r="D55" s="2" t="s">
         <v>62</v>
       </c>
@@ -15557,7 +15559,7 @@
         <v>20</v>
       </c>
       <c r="K55" s="34" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="L55" s="34"/>
       <c r="M55" s="34"/>
@@ -15585,8 +15587,8 @@
     </row>
     <row r="56" spans="1:30">
       <c r="A56" s="3"/>
-      <c r="B56" s="48"/>
-      <c r="C56" s="48"/>
+      <c r="B56" s="49"/>
+      <c r="C56" s="49"/>
       <c r="D56" s="2" t="s">
         <v>63</v>
       </c>
@@ -15603,7 +15605,7 @@
         <v>20</v>
       </c>
       <c r="K56" s="34" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="L56" s="34"/>
       <c r="M56" s="34"/>
@@ -15631,10 +15633,10 @@
     </row>
     <row r="57" spans="1:30" ht="18" customHeight="1">
       <c r="A57" s="3"/>
-      <c r="B57" s="46" t="s">
+      <c r="B57" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="C57" s="46"/>
+      <c r="C57" s="47"/>
       <c r="D57" s="1" t="s">
         <v>65</v>
       </c>
@@ -15651,7 +15653,7 @@
         <v>20</v>
       </c>
       <c r="K57" s="34" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="L57" s="34"/>
       <c r="M57" s="34"/>
@@ -15659,7 +15661,7 @@
         <v>276</v>
       </c>
       <c r="O57" s="19" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="P57" s="19"/>
       <c r="Q57" s="19"/>
@@ -15679,8 +15681,8 @@
     </row>
     <row r="58" spans="1:30">
       <c r="A58" s="3"/>
-      <c r="B58" s="46"/>
-      <c r="C58" s="46"/>
+      <c r="B58" s="47"/>
+      <c r="C58" s="47"/>
       <c r="D58" s="1" t="s">
         <v>66</v>
       </c>
@@ -15697,7 +15699,7 @@
         <v>20</v>
       </c>
       <c r="K58" s="34" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="L58" s="34"/>
       <c r="M58" s="34"/>
@@ -15725,8 +15727,8 @@
     </row>
     <row r="59" spans="1:30">
       <c r="A59" s="3"/>
-      <c r="B59" s="46"/>
-      <c r="C59" s="46"/>
+      <c r="B59" s="47"/>
+      <c r="C59" s="47"/>
       <c r="D59" s="1" t="s">
         <v>67</v>
       </c>
@@ -15765,8 +15767,8 @@
     </row>
     <row r="60" spans="1:30">
       <c r="A60" s="3"/>
-      <c r="B60" s="46"/>
-      <c r="C60" s="46"/>
+      <c r="B60" s="47"/>
+      <c r="C60" s="47"/>
       <c r="D60" s="1" t="s">
         <v>68</v>
       </c>
@@ -15783,7 +15785,7 @@
         <v>20</v>
       </c>
       <c r="K60" s="34" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="L60" s="34"/>
       <c r="M60" s="34"/>
@@ -15811,8 +15813,8 @@
     </row>
     <row r="61" spans="1:30">
       <c r="A61" s="3"/>
-      <c r="B61" s="46"/>
-      <c r="C61" s="46"/>
+      <c r="B61" s="47"/>
+      <c r="C61" s="47"/>
       <c r="D61" s="1" t="s">
         <v>69</v>
       </c>
@@ -15829,7 +15831,7 @@
         <v>20</v>
       </c>
       <c r="K61" s="34" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="L61" s="34"/>
       <c r="M61" s="34"/>
@@ -15953,13 +15955,13 @@
     </row>
     <row r="65" spans="1:30" ht="18" customHeight="1">
       <c r="A65" s="3"/>
-      <c r="B65" s="44" t="s">
+      <c r="B65" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="C65" s="44"/>
-      <c r="D65" s="44"/>
-      <c r="E65" s="44"/>
-      <c r="F65" s="44"/>
+      <c r="C65" s="45"/>
+      <c r="D65" s="45"/>
+      <c r="E65" s="45"/>
+      <c r="F65" s="45"/>
       <c r="G65" s="3"/>
       <c r="H65" s="3"/>
       <c r="I65" s="3"/>
@@ -15987,11 +15989,11 @@
     </row>
     <row r="66" spans="1:30">
       <c r="A66" s="3"/>
-      <c r="B66" s="44"/>
-      <c r="C66" s="44"/>
-      <c r="D66" s="44"/>
-      <c r="E66" s="44"/>
-      <c r="F66" s="44"/>
+      <c r="B66" s="45"/>
+      <c r="C66" s="45"/>
+      <c r="D66" s="45"/>
+      <c r="E66" s="45"/>
+      <c r="F66" s="45"/>
       <c r="G66" s="3"/>
       <c r="H66" s="3"/>
       <c r="I66" s="3"/>
@@ -46477,10 +46479,10 @@
       </c>
     </row>
     <row r="6" spans="4:6" ht="26" thickTop="1">
-      <c r="D6" s="57">
+      <c r="D6" s="58">
         <v>1</v>
       </c>
-      <c r="E6" s="57" t="s">
+      <c r="E6" s="58" t="s">
         <v>77</v>
       </c>
       <c r="F6" s="13" t="s">
@@ -46488,24 +46490,24 @@
       </c>
     </row>
     <row r="7" spans="4:6">
-      <c r="D7" s="58"/>
-      <c r="E7" s="58"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="59"/>
       <c r="F7" s="12" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="8" spans="4:6" ht="26">
-      <c r="D8" s="58"/>
-      <c r="E8" s="58"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="59"/>
       <c r="F8" s="12" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="9" spans="4:6" ht="25.5">
-      <c r="D9" s="57">
+      <c r="D9" s="58">
         <v>2</v>
       </c>
-      <c r="E9" s="57" t="s">
+      <c r="E9" s="58" t="s">
         <v>79</v>
       </c>
       <c r="F9" s="13" t="s">
@@ -46513,24 +46515,24 @@
       </c>
     </row>
     <row r="10" spans="4:6">
-      <c r="D10" s="58"/>
-      <c r="E10" s="58"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="59"/>
       <c r="F10" s="12" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="11" spans="4:6">
-      <c r="D11" s="58"/>
-      <c r="E11" s="58"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="59"/>
       <c r="F11" s="12" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="12" spans="4:6">
-      <c r="D12" s="57">
+      <c r="D12" s="58">
         <v>3</v>
       </c>
-      <c r="E12" s="57" t="s">
+      <c r="E12" s="58" t="s">
         <v>128</v>
       </c>
       <c r="F12" s="13" t="s">
@@ -46538,24 +46540,24 @@
       </c>
     </row>
     <row r="13" spans="4:6">
-      <c r="D13" s="58"/>
-      <c r="E13" s="58"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="59"/>
       <c r="F13" s="12" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="14" spans="4:6">
-      <c r="D14" s="58"/>
-      <c r="E14" s="58"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="59"/>
       <c r="F14" s="12" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="15" spans="4:6" ht="25">
-      <c r="D15" s="57">
+      <c r="D15" s="58">
         <v>4</v>
       </c>
-      <c r="E15" s="57" t="s">
+      <c r="E15" s="58" t="s">
         <v>129</v>
       </c>
       <c r="F15" s="13" t="s">
@@ -46563,24 +46565,24 @@
       </c>
     </row>
     <row r="16" spans="4:6" ht="26">
-      <c r="D16" s="58"/>
-      <c r="E16" s="58"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="59"/>
       <c r="F16" s="12" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="17" spans="4:6">
-      <c r="D17" s="58"/>
-      <c r="E17" s="58"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="59"/>
       <c r="F17" s="12" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="18" spans="4:6" ht="38">
-      <c r="D18" s="57">
+      <c r="D18" s="58">
         <v>5</v>
       </c>
-      <c r="E18" s="57" t="s">
+      <c r="E18" s="58" t="s">
         <v>130</v>
       </c>
       <c r="F18" s="13" t="s">
@@ -46588,24 +46590,24 @@
       </c>
     </row>
     <row r="19" spans="4:6">
-      <c r="D19" s="58"/>
-      <c r="E19" s="58"/>
+      <c r="D19" s="59"/>
+      <c r="E19" s="59"/>
       <c r="F19" s="12" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="20" spans="4:6">
-      <c r="D20" s="58"/>
-      <c r="E20" s="58"/>
+      <c r="D20" s="59"/>
+      <c r="E20" s="59"/>
       <c r="F20" s="12" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="21" spans="4:6">
-      <c r="D21" s="57">
+      <c r="D21" s="58">
         <v>6</v>
       </c>
-      <c r="E21" s="57" t="s">
+      <c r="E21" s="58" t="s">
         <v>90</v>
       </c>
       <c r="F21" s="13" t="s">
@@ -46613,24 +46615,24 @@
       </c>
     </row>
     <row r="22" spans="4:6">
-      <c r="D22" s="58"/>
-      <c r="E22" s="58"/>
+      <c r="D22" s="59"/>
+      <c r="E22" s="59"/>
       <c r="F22" s="12" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="23" spans="4:6">
-      <c r="D23" s="58"/>
-      <c r="E23" s="58"/>
+      <c r="D23" s="59"/>
+      <c r="E23" s="59"/>
       <c r="F23" s="12" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="24" spans="4:6" ht="38">
-      <c r="D24" s="57">
+      <c r="D24" s="58">
         <v>7</v>
       </c>
-      <c r="E24" s="57" t="s">
+      <c r="E24" s="58" t="s">
         <v>129</v>
       </c>
       <c r="F24" s="13" t="s">
@@ -46638,24 +46640,24 @@
       </c>
     </row>
     <row r="25" spans="4:6">
-      <c r="D25" s="58"/>
-      <c r="E25" s="58"/>
+      <c r="D25" s="59"/>
+      <c r="E25" s="59"/>
       <c r="F25" s="12" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="26" spans="4:6">
-      <c r="D26" s="58"/>
-      <c r="E26" s="58"/>
+      <c r="D26" s="59"/>
+      <c r="E26" s="59"/>
       <c r="F26" s="12" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="27" spans="4:6" ht="26">
-      <c r="D27" s="57">
+      <c r="D27" s="58">
         <v>8</v>
       </c>
-      <c r="E27" s="57" t="s">
+      <c r="E27" s="58" t="s">
         <v>131</v>
       </c>
       <c r="F27" s="13" t="s">
@@ -46663,24 +46665,24 @@
       </c>
     </row>
     <row r="28" spans="4:6" ht="26">
-      <c r="D28" s="58"/>
-      <c r="E28" s="58"/>
+      <c r="D28" s="59"/>
+      <c r="E28" s="59"/>
       <c r="F28" s="12" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="29" spans="4:6">
-      <c r="D29" s="58"/>
-      <c r="E29" s="58"/>
+      <c r="D29" s="59"/>
+      <c r="E29" s="59"/>
       <c r="F29" s="12" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="30" spans="4:6" ht="25">
-      <c r="D30" s="57">
+      <c r="D30" s="58">
         <v>9</v>
       </c>
-      <c r="E30" s="57" t="s">
+      <c r="E30" s="58" t="s">
         <v>79</v>
       </c>
       <c r="F30" s="13" t="s">
@@ -46688,24 +46690,24 @@
       </c>
     </row>
     <row r="31" spans="4:6">
-      <c r="D31" s="58"/>
-      <c r="E31" s="58"/>
+      <c r="D31" s="59"/>
+      <c r="E31" s="59"/>
       <c r="F31" s="12" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="32" spans="4:6">
-      <c r="D32" s="58"/>
-      <c r="E32" s="58"/>
+      <c r="D32" s="59"/>
+      <c r="E32" s="59"/>
       <c r="F32" s="12" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="33" spans="4:6">
-      <c r="D33" s="57">
+      <c r="D33" s="58">
         <v>10</v>
       </c>
-      <c r="E33" s="57" t="s">
+      <c r="E33" s="58" t="s">
         <v>79</v>
       </c>
       <c r="F33" s="13" t="s">
@@ -46713,24 +46715,24 @@
       </c>
     </row>
     <row r="34" spans="4:6">
-      <c r="D34" s="58"/>
-      <c r="E34" s="58"/>
+      <c r="D34" s="59"/>
+      <c r="E34" s="59"/>
       <c r="F34" s="12" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="35" spans="4:6">
-      <c r="D35" s="58"/>
-      <c r="E35" s="58"/>
+      <c r="D35" s="59"/>
+      <c r="E35" s="59"/>
       <c r="F35" s="12" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="36" spans="4:6" ht="25">
-      <c r="D36" s="57">
+      <c r="D36" s="58">
         <v>11</v>
       </c>
-      <c r="E36" s="57" t="s">
+      <c r="E36" s="58" t="s">
         <v>132</v>
       </c>
       <c r="F36" s="13" t="s">
@@ -46738,24 +46740,24 @@
       </c>
     </row>
     <row r="37" spans="4:6">
-      <c r="D37" s="58"/>
-      <c r="E37" s="58"/>
+      <c r="D37" s="59"/>
+      <c r="E37" s="59"/>
       <c r="F37" s="12" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="38" spans="4:6">
-      <c r="D38" s="58"/>
-      <c r="E38" s="58"/>
+      <c r="D38" s="59"/>
+      <c r="E38" s="59"/>
       <c r="F38" s="12" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="39" spans="4:6" ht="37.5">
-      <c r="D39" s="57">
+      <c r="D39" s="58">
         <v>12</v>
       </c>
-      <c r="E39" s="57" t="s">
+      <c r="E39" s="58" t="s">
         <v>133</v>
       </c>
       <c r="F39" s="13" t="s">
@@ -46763,24 +46765,24 @@
       </c>
     </row>
     <row r="40" spans="4:6">
-      <c r="D40" s="58"/>
-      <c r="E40" s="58"/>
+      <c r="D40" s="59"/>
+      <c r="E40" s="59"/>
       <c r="F40" s="12" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="41" spans="4:6">
-      <c r="D41" s="58"/>
-      <c r="E41" s="58"/>
+      <c r="D41" s="59"/>
+      <c r="E41" s="59"/>
       <c r="F41" s="12" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="42" spans="4:6" ht="25">
-      <c r="D42" s="57">
+      <c r="D42" s="58">
         <v>13</v>
       </c>
-      <c r="E42" s="57" t="s">
+      <c r="E42" s="58" t="s">
         <v>129</v>
       </c>
       <c r="F42" s="13" t="s">
@@ -46788,24 +46790,24 @@
       </c>
     </row>
     <row r="43" spans="4:6">
-      <c r="D43" s="58"/>
-      <c r="E43" s="58"/>
+      <c r="D43" s="59"/>
+      <c r="E43" s="59"/>
       <c r="F43" s="12" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="44" spans="4:6">
-      <c r="D44" s="58"/>
-      <c r="E44" s="58"/>
+      <c r="D44" s="59"/>
+      <c r="E44" s="59"/>
       <c r="F44" s="12" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="45" spans="4:6" ht="75.5">
-      <c r="D45" s="57">
+      <c r="D45" s="58">
         <v>14</v>
       </c>
-      <c r="E45" s="57" t="s">
+      <c r="E45" s="58" t="s">
         <v>134</v>
       </c>
       <c r="F45" s="13" t="s">
@@ -46813,24 +46815,24 @@
       </c>
     </row>
     <row r="46" spans="4:6" ht="26">
-      <c r="D46" s="58"/>
-      <c r="E46" s="58"/>
+      <c r="D46" s="59"/>
+      <c r="E46" s="59"/>
       <c r="F46" s="12" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="47" spans="4:6">
-      <c r="D47" s="58"/>
-      <c r="E47" s="58"/>
+      <c r="D47" s="59"/>
+      <c r="E47" s="59"/>
       <c r="F47" s="12" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="48" spans="4:6" ht="37.5">
-      <c r="D48" s="57">
+      <c r="D48" s="58">
         <v>15</v>
       </c>
-      <c r="E48" s="57" t="s">
+      <c r="E48" s="58" t="s">
         <v>135</v>
       </c>
       <c r="F48" s="13" t="s">
@@ -46838,24 +46840,24 @@
       </c>
     </row>
     <row r="49" spans="4:6" ht="26">
-      <c r="D49" s="58"/>
-      <c r="E49" s="58"/>
+      <c r="D49" s="59"/>
+      <c r="E49" s="59"/>
       <c r="F49" s="12" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="50" spans="4:6">
-      <c r="D50" s="58"/>
-      <c r="E50" s="58"/>
+      <c r="D50" s="59"/>
+      <c r="E50" s="59"/>
       <c r="F50" s="12" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="51" spans="4:6" ht="25">
-      <c r="D51" s="57">
+      <c r="D51" s="58">
         <v>16</v>
       </c>
-      <c r="E51" s="57" t="s">
+      <c r="E51" s="58" t="s">
         <v>136</v>
       </c>
       <c r="F51" s="13" t="s">
@@ -46863,24 +46865,24 @@
       </c>
     </row>
     <row r="52" spans="4:6">
-      <c r="D52" s="58"/>
-      <c r="E52" s="58"/>
+      <c r="D52" s="59"/>
+      <c r="E52" s="59"/>
       <c r="F52" s="12" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="53" spans="4:6">
-      <c r="D53" s="58"/>
-      <c r="E53" s="58"/>
+      <c r="D53" s="59"/>
+      <c r="E53" s="59"/>
       <c r="F53" s="12" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="54" spans="4:6" ht="25">
-      <c r="D54" s="57">
+      <c r="D54" s="58">
         <v>17</v>
       </c>
-      <c r="E54" s="57" t="s">
+      <c r="E54" s="58" t="s">
         <v>136</v>
       </c>
       <c r="F54" s="13" t="s">
@@ -46888,24 +46890,24 @@
       </c>
     </row>
     <row r="55" spans="4:6">
-      <c r="D55" s="58"/>
-      <c r="E55" s="58"/>
+      <c r="D55" s="59"/>
+      <c r="E55" s="59"/>
       <c r="F55" s="12" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="56" spans="4:6">
-      <c r="D56" s="58"/>
-      <c r="E56" s="58"/>
+      <c r="D56" s="59"/>
+      <c r="E56" s="59"/>
       <c r="F56" s="12" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="57" spans="4:6">
-      <c r="D57" s="57">
+      <c r="D57" s="58">
         <v>18</v>
       </c>
-      <c r="E57" s="57" t="s">
+      <c r="E57" s="58" t="s">
         <v>79</v>
       </c>
       <c r="F57" s="13" t="s">
@@ -46913,24 +46915,24 @@
       </c>
     </row>
     <row r="58" spans="4:6">
-      <c r="D58" s="58"/>
-      <c r="E58" s="58"/>
+      <c r="D58" s="59"/>
+      <c r="E58" s="59"/>
       <c r="F58" s="12" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="59" spans="4:6">
-      <c r="D59" s="58"/>
-      <c r="E59" s="58"/>
+      <c r="D59" s="59"/>
+      <c r="E59" s="59"/>
       <c r="F59" s="12" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="60" spans="4:6" ht="34">
-      <c r="D60" s="57">
+      <c r="D60" s="58">
         <v>19</v>
       </c>
-      <c r="E60" s="57" t="s">
+      <c r="E60" s="58" t="s">
         <v>79</v>
       </c>
       <c r="F60" s="16" t="s">
@@ -46938,24 +46940,24 @@
       </c>
     </row>
     <row r="61" spans="4:6">
-      <c r="D61" s="58"/>
-      <c r="E61" s="58"/>
+      <c r="D61" s="59"/>
+      <c r="E61" s="59"/>
       <c r="F61" s="12" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="62" spans="4:6">
-      <c r="D62" s="58"/>
-      <c r="E62" s="58"/>
+      <c r="D62" s="59"/>
+      <c r="E62" s="59"/>
       <c r="F62" s="12" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="63" spans="4:6" ht="34">
-      <c r="D63" s="57">
+      <c r="D63" s="58">
         <v>20</v>
       </c>
-      <c r="E63" s="57" t="s">
+      <c r="E63" s="58" t="s">
         <v>81</v>
       </c>
       <c r="F63" s="16" t="s">
@@ -46963,24 +46965,24 @@
       </c>
     </row>
     <row r="64" spans="4:6">
-      <c r="D64" s="58"/>
-      <c r="E64" s="58"/>
+      <c r="D64" s="59"/>
+      <c r="E64" s="59"/>
       <c r="F64" s="12" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="65" spans="4:6">
-      <c r="D65" s="58"/>
-      <c r="E65" s="58"/>
+      <c r="D65" s="59"/>
+      <c r="E65" s="59"/>
       <c r="F65" s="12" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="66" spans="4:6" ht="34">
-      <c r="D66" s="57">
+      <c r="D66" s="58">
         <v>21</v>
       </c>
-      <c r="E66" s="57" t="s">
+      <c r="E66" s="58" t="s">
         <v>81</v>
       </c>
       <c r="F66" s="16" t="s">
@@ -46988,24 +46990,24 @@
       </c>
     </row>
     <row r="67" spans="4:6" ht="26">
-      <c r="D67" s="58"/>
-      <c r="E67" s="58"/>
+      <c r="D67" s="59"/>
+      <c r="E67" s="59"/>
       <c r="F67" s="12" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="68" spans="4:6">
-      <c r="D68" s="58"/>
-      <c r="E68" s="58"/>
+      <c r="D68" s="59"/>
+      <c r="E68" s="59"/>
       <c r="F68" s="12" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="69" spans="4:6" ht="34">
-      <c r="D69" s="57">
+      <c r="D69" s="58">
         <v>22</v>
       </c>
-      <c r="E69" s="57" t="s">
+      <c r="E69" s="58" t="s">
         <v>90</v>
       </c>
       <c r="F69" s="16" t="s">
@@ -47013,24 +47015,24 @@
       </c>
     </row>
     <row r="70" spans="4:6" ht="26">
-      <c r="D70" s="58"/>
-      <c r="E70" s="58"/>
+      <c r="D70" s="59"/>
+      <c r="E70" s="59"/>
       <c r="F70" s="12" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="71" spans="4:6">
-      <c r="D71" s="58"/>
-      <c r="E71" s="58"/>
+      <c r="D71" s="59"/>
+      <c r="E71" s="59"/>
       <c r="F71" s="12" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="72" spans="4:6">
-      <c r="D72" s="57">
+      <c r="D72" s="58">
         <v>23</v>
       </c>
-      <c r="E72" s="57" t="s">
+      <c r="E72" s="58" t="s">
         <v>112</v>
       </c>
       <c r="F72" s="5" t="s">
@@ -47038,24 +47040,24 @@
       </c>
     </row>
     <row r="73" spans="4:6" ht="26">
-      <c r="D73" s="58"/>
-      <c r="E73" s="58"/>
+      <c r="D73" s="59"/>
+      <c r="E73" s="59"/>
       <c r="F73" s="12" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="74" spans="4:6">
-      <c r="D74" s="58"/>
-      <c r="E74" s="58"/>
+      <c r="D74" s="59"/>
+      <c r="E74" s="59"/>
       <c r="F74" s="12" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="75" spans="4:6">
-      <c r="D75" s="57">
+      <c r="D75" s="58">
         <v>24</v>
       </c>
-      <c r="E75" s="57" t="s">
+      <c r="E75" s="58" t="s">
         <v>79</v>
       </c>
       <c r="F75" s="15" t="s">
@@ -47063,24 +47065,24 @@
       </c>
     </row>
     <row r="76" spans="4:6">
-      <c r="D76" s="58"/>
-      <c r="E76" s="58"/>
+      <c r="D76" s="59"/>
+      <c r="E76" s="59"/>
       <c r="F76" s="12" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="77" spans="4:6">
-      <c r="D77" s="58"/>
-      <c r="E77" s="58"/>
+      <c r="D77" s="59"/>
+      <c r="E77" s="59"/>
       <c r="F77" s="12" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="78" spans="4:6" ht="34">
-      <c r="D78" s="57">
+      <c r="D78" s="58">
         <v>25</v>
       </c>
-      <c r="E78" s="57" t="s">
+      <c r="E78" s="58" t="s">
         <v>79</v>
       </c>
       <c r="F78" s="16" t="s">
@@ -47088,55 +47090,21 @@
       </c>
     </row>
     <row r="79" spans="4:6">
-      <c r="D79" s="58"/>
-      <c r="E79" s="58"/>
+      <c r="D79" s="59"/>
+      <c r="E79" s="59"/>
       <c r="F79" s="12" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="80" spans="4:6">
-      <c r="D80" s="58"/>
-      <c r="E80" s="58"/>
+      <c r="D80" s="59"/>
+      <c r="E80" s="59"/>
       <c r="F80" s="12" t="s">
         <v>177</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="D60:D62"/>
-    <mergeCell ref="E60:E62"/>
-    <mergeCell ref="D72:D74"/>
-    <mergeCell ref="E72:E74"/>
-    <mergeCell ref="D63:D65"/>
-    <mergeCell ref="E63:E65"/>
-    <mergeCell ref="D66:D68"/>
-    <mergeCell ref="E66:E68"/>
-    <mergeCell ref="D69:D71"/>
-    <mergeCell ref="E69:E71"/>
-    <mergeCell ref="D51:D53"/>
-    <mergeCell ref="E51:E53"/>
-    <mergeCell ref="D54:D56"/>
-    <mergeCell ref="E54:E56"/>
-    <mergeCell ref="D57:D59"/>
-    <mergeCell ref="E57:E59"/>
-    <mergeCell ref="D42:D44"/>
-    <mergeCell ref="E42:E44"/>
-    <mergeCell ref="D45:D47"/>
-    <mergeCell ref="E45:E47"/>
-    <mergeCell ref="D48:D50"/>
-    <mergeCell ref="E48:E50"/>
-    <mergeCell ref="D33:D35"/>
-    <mergeCell ref="E33:E35"/>
-    <mergeCell ref="D36:D38"/>
-    <mergeCell ref="E36:E38"/>
-    <mergeCell ref="D39:D41"/>
-    <mergeCell ref="E39:E41"/>
-    <mergeCell ref="D24:D26"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="D27:D29"/>
-    <mergeCell ref="E27:E29"/>
-    <mergeCell ref="D30:D32"/>
-    <mergeCell ref="E30:E32"/>
     <mergeCell ref="D75:D77"/>
     <mergeCell ref="E75:E77"/>
     <mergeCell ref="D78:D80"/>
@@ -47153,6 +47121,40 @@
     <mergeCell ref="E18:E20"/>
     <mergeCell ref="D21:D23"/>
     <mergeCell ref="E21:E23"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="D27:D29"/>
+    <mergeCell ref="E27:E29"/>
+    <mergeCell ref="D30:D32"/>
+    <mergeCell ref="E30:E32"/>
+    <mergeCell ref="D33:D35"/>
+    <mergeCell ref="E33:E35"/>
+    <mergeCell ref="D36:D38"/>
+    <mergeCell ref="E36:E38"/>
+    <mergeCell ref="D39:D41"/>
+    <mergeCell ref="E39:E41"/>
+    <mergeCell ref="D42:D44"/>
+    <mergeCell ref="E42:E44"/>
+    <mergeCell ref="D45:D47"/>
+    <mergeCell ref="E45:E47"/>
+    <mergeCell ref="D48:D50"/>
+    <mergeCell ref="E48:E50"/>
+    <mergeCell ref="D51:D53"/>
+    <mergeCell ref="E51:E53"/>
+    <mergeCell ref="D54:D56"/>
+    <mergeCell ref="E54:E56"/>
+    <mergeCell ref="D57:D59"/>
+    <mergeCell ref="E57:E59"/>
+    <mergeCell ref="D60:D62"/>
+    <mergeCell ref="E60:E62"/>
+    <mergeCell ref="D72:D74"/>
+    <mergeCell ref="E72:E74"/>
+    <mergeCell ref="D63:D65"/>
+    <mergeCell ref="E63:E65"/>
+    <mergeCell ref="D66:D68"/>
+    <mergeCell ref="E66:E68"/>
+    <mergeCell ref="D69:D71"/>
+    <mergeCell ref="E69:E71"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>